<commit_message>
improve calendar month look
</commit_message>
<xml_diff>
--- a/schedule_5_2025.xlsx
+++ b/schedule_5_2025.xlsx
@@ -16,14 +16,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="201">
   <si>
     <t>May 2025</t>
   </si>
   <si>
-    <t>Time Slot</t>
-  </si>
-  <si>
     <t>Mon</t>
   </si>
   <si>
@@ -48,19 +45,19 @@
     <t>9AM-11AM</t>
   </si>
   <si>
+    <t>11AM-1PM</t>
+  </si>
+  <si>
+    <t>1PM-3PM</t>
+  </si>
+  <si>
+    <t>3PM-5PM</t>
+  </si>
+  <si>
     <t>R C</t>
   </si>
   <si>
     <t>b b</t>
-  </si>
-  <si>
-    <t>11AM-1PM</t>
-  </si>
-  <si>
-    <t>1PM-3PM</t>
-  </si>
-  <si>
-    <t>3PM-5PM</t>
   </si>
   <si>
     <t>Name</t>
@@ -628,7 +625,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -651,7 +648,14 @@
       <family val="2"/>
     </font>
     <font>
+      <b/>
       <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -664,7 +668,6 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
@@ -679,7 +682,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -694,7 +697,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FFC0C0C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA9A9A9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -726,7 +735,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -734,23 +743,26 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -1047,17 +1059,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I67"/>
+  <dimension ref="A1:O62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" customWidth="1"/>
-    <col min="2" max="8" width="18.7109375" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="2" max="2" width="4.7109375" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" customWidth="1"/>
+    <col min="4" max="4" width="4.7109375" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" customWidth="1"/>
+    <col min="6" max="6" width="4.7109375" customWidth="1"/>
+    <col min="7" max="7" width="18.7109375" customWidth="1"/>
+    <col min="8" max="8" width="4.7109375" customWidth="1"/>
+    <col min="9" max="9" width="18.7109375" customWidth="1"/>
+    <col min="10" max="10" width="4.7109375" customWidth="1"/>
+    <col min="11" max="11" width="18.7109375" customWidth="1"/>
+    <col min="12" max="12" width="4.7109375" customWidth="1"/>
+    <col min="13" max="13" width="18.7109375" customWidth="1"/>
+    <col min="14" max="14" width="4.7109375" customWidth="1"/>
+    <col min="15" max="15" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1069,1023 +1094,1450 @@
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
-    </row>
-    <row r="2" spans="1:9">
-      <c r="A2" s="2" t="s">
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+    </row>
+    <row r="2" spans="1:15" ht="20" customHeight="1">
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2"/>
+      <c r="D2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="E2" s="2"/>
+      <c r="F2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="G2" s="2"/>
+      <c r="H2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="I2" s="2"/>
+      <c r="J2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="K2" s="2"/>
+      <c r="L2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="M2" s="2"/>
+      <c r="N2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="O2" s="2"/>
+    </row>
+    <row r="3" spans="1:15">
+      <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" ht="24" customHeight="1">
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="4">
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="5">
         <v>1</v>
       </c>
-      <c r="F3" s="4">
+      <c r="I3" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="J3" s="5">
         <v>2</v>
       </c>
-      <c r="G3" s="4">
+      <c r="K3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="L3" s="5">
         <v>3</v>
       </c>
-      <c r="H3" s="4">
+      <c r="M3" s="6"/>
+      <c r="N3" s="5">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" s="5" t="s">
+      <c r="O3" s="6"/>
+    </row>
+    <row r="4" spans="1:15">
+      <c r="A4" s="3"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J4" s="5"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="6"/>
+      <c r="N4" s="5"/>
+      <c r="O4" s="6"/>
+    </row>
+    <row r="5" spans="1:15">
+      <c r="A5" s="3"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="5"/>
+      <c r="O5" s="6"/>
+    </row>
+    <row r="6" spans="1:15">
+      <c r="A6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3" t="s">
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="J6" s="5"/>
+      <c r="K6" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="L6" s="5"/>
+      <c r="M6" s="7"/>
+      <c r="N6" s="5"/>
+      <c r="O6" s="7"/>
+    </row>
+    <row r="7" spans="1:15">
+      <c r="A7" s="3"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="L7" s="5"/>
+      <c r="M7" s="7"/>
+      <c r="N7" s="5"/>
+      <c r="O7" s="7"/>
+    </row>
+    <row r="8" spans="1:15">
+      <c r="A8" s="3"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="7"/>
+      <c r="N8" s="5"/>
+      <c r="O8" s="7"/>
+    </row>
+    <row r="9" spans="1:15">
+      <c r="A9" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J9" s="5"/>
+      <c r="K9" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="L9" s="5"/>
+      <c r="M9" s="6"/>
+      <c r="N9" s="5"/>
+      <c r="O9" s="6"/>
+    </row>
+    <row r="10" spans="1:15">
+      <c r="A10" s="3"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="5"/>
+      <c r="O10" s="6"/>
+    </row>
+    <row r="11" spans="1:15">
+      <c r="A11" s="3"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="6"/>
+      <c r="N11" s="5"/>
+      <c r="O11" s="6"/>
+    </row>
+    <row r="12" spans="1:15">
+      <c r="A12" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5" s="5"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3" t="s">
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="J12" s="5"/>
+      <c r="K12" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="L12" s="5"/>
+      <c r="M12" s="7"/>
+      <c r="N12" s="5"/>
+      <c r="O12" s="7"/>
+    </row>
+    <row r="13" spans="1:15">
+      <c r="A13" s="3"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="7"/>
+      <c r="L13" s="5"/>
+      <c r="M13" s="7"/>
+      <c r="N13" s="5"/>
+      <c r="O13" s="7"/>
+    </row>
+    <row r="14" spans="1:15">
+      <c r="A14" s="3"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="7"/>
+      <c r="L14" s="5"/>
+      <c r="M14" s="7"/>
+      <c r="N14" s="5"/>
+      <c r="O14" s="7"/>
+    </row>
+    <row r="15" spans="1:15">
+      <c r="A15" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" s="5">
+        <v>5</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" s="5">
+        <v>6</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F15" s="5">
+        <v>7</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H15" s="5">
+        <v>8</v>
+      </c>
+      <c r="I15" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="J15" s="5">
+        <v>9</v>
+      </c>
+      <c r="K15" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="L15" s="5">
+        <v>10</v>
+      </c>
+      <c r="M15" s="6"/>
+      <c r="N15" s="5">
         <v>11</v>
       </c>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="A6" s="5"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7" s="6" t="s">
+      <c r="O15" s="6"/>
+    </row>
+    <row r="16" spans="1:15">
+      <c r="A16" s="8"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J16" s="5"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="5"/>
+      <c r="M16" s="6"/>
+      <c r="N16" s="5"/>
+      <c r="O16" s="6"/>
+    </row>
+    <row r="17" spans="1:15">
+      <c r="A17" s="8"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="6"/>
+      <c r="L17" s="5"/>
+      <c r="M17" s="6"/>
+      <c r="N17" s="5"/>
+      <c r="O17" s="6"/>
+    </row>
+    <row r="18" spans="1:15">
+      <c r="A18" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" s="5"/>
+      <c r="C18" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" s="5"/>
+      <c r="E18" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F18" s="5"/>
+      <c r="G18" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H18" s="5"/>
+      <c r="I18" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="J18" s="5"/>
+      <c r="K18" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7" t="s">
+      <c r="L18" s="5"/>
+      <c r="M18" s="7"/>
+      <c r="N18" s="5"/>
+      <c r="O18" s="7"/>
+    </row>
+    <row r="19" spans="1:15">
+      <c r="A19" s="8"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="L19" s="5"/>
+      <c r="M19" s="7"/>
+      <c r="N19" s="5"/>
+      <c r="O19" s="7"/>
+    </row>
+    <row r="20" spans="1:15">
+      <c r="A20" s="8"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="5"/>
+      <c r="K20" s="7"/>
+      <c r="L20" s="5"/>
+      <c r="M20" s="7"/>
+      <c r="N20" s="5"/>
+      <c r="O20" s="7"/>
+    </row>
+    <row r="21" spans="1:15">
+      <c r="A21" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B21" s="5"/>
+      <c r="C21" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D21" s="5"/>
+      <c r="E21" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F21" s="5"/>
+      <c r="G21" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H21" s="5"/>
+      <c r="I21" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J21" s="5"/>
+      <c r="K21" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="L21" s="5"/>
+      <c r="M21" s="6"/>
+      <c r="N21" s="5"/>
+      <c r="O21" s="6"/>
+    </row>
+    <row r="22" spans="1:15">
+      <c r="A22" s="8"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F22" s="5"/>
+      <c r="G22" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H22" s="5"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="6"/>
+      <c r="L22" s="5"/>
+      <c r="M22" s="6"/>
+      <c r="N22" s="5"/>
+      <c r="O22" s="6"/>
+    </row>
+    <row r="23" spans="1:15">
+      <c r="A23" s="8"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="6"/>
+      <c r="L23" s="5"/>
+      <c r="M23" s="6"/>
+      <c r="N23" s="5"/>
+      <c r="O23" s="6"/>
+    </row>
+    <row r="24" spans="1:15">
+      <c r="A24" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="B24" s="5"/>
+      <c r="C24" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D24" s="5"/>
+      <c r="E24" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F24" s="5"/>
+      <c r="G24" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H24" s="5"/>
+      <c r="I24" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="J24" s="5"/>
+      <c r="K24" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="L24" s="5"/>
+      <c r="M24" s="7"/>
+      <c r="N24" s="5"/>
+      <c r="O24" s="7"/>
+    </row>
+    <row r="25" spans="1:15">
+      <c r="A25" s="8"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D25" s="5"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="7"/>
+      <c r="J25" s="5"/>
+      <c r="K25" s="7"/>
+      <c r="L25" s="5"/>
+      <c r="M25" s="7"/>
+      <c r="N25" s="5"/>
+      <c r="O25" s="7"/>
+    </row>
+    <row r="26" spans="1:15">
+      <c r="A26" s="8"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="7"/>
+      <c r="H26" s="5"/>
+      <c r="I26" s="7"/>
+      <c r="J26" s="5"/>
+      <c r="K26" s="7"/>
+      <c r="L26" s="5"/>
+      <c r="M26" s="7"/>
+      <c r="N26" s="5"/>
+      <c r="O26" s="7"/>
+    </row>
+    <row r="27" spans="1:15">
+      <c r="A27" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B27" s="5">
+        <v>12</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D27" s="5">
+        <v>13</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F27" s="5">
+        <v>14</v>
+      </c>
+      <c r="G27" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H27" s="5">
+        <v>15</v>
+      </c>
+      <c r="I27" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="J27" s="5">
+        <v>16</v>
+      </c>
+      <c r="K27" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="L27" s="5">
+        <v>17</v>
+      </c>
+      <c r="M27" s="6"/>
+      <c r="N27" s="5">
+        <v>18</v>
+      </c>
+      <c r="O27" s="6"/>
+    </row>
+    <row r="28" spans="1:15">
+      <c r="A28" s="3"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="6"/>
+      <c r="H28" s="5"/>
+      <c r="I28" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J28" s="5"/>
+      <c r="K28" s="6"/>
+      <c r="L28" s="5"/>
+      <c r="M28" s="6"/>
+      <c r="N28" s="5"/>
+      <c r="O28" s="6"/>
+    </row>
+    <row r="29" spans="1:15">
+      <c r="A29" s="3"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="5"/>
+      <c r="I29" s="6"/>
+      <c r="J29" s="5"/>
+      <c r="K29" s="6"/>
+      <c r="L29" s="5"/>
+      <c r="M29" s="6"/>
+      <c r="N29" s="5"/>
+      <c r="O29" s="6"/>
+    </row>
+    <row r="30" spans="1:15">
+      <c r="A30" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B30" s="5"/>
+      <c r="C30" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D30" s="5"/>
+      <c r="E30" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F30" s="5"/>
+      <c r="G30" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H30" s="5"/>
+      <c r="I30" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="J30" s="5"/>
+      <c r="K30" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="L30" s="5"/>
+      <c r="M30" s="7"/>
+      <c r="N30" s="5"/>
+      <c r="O30" s="7"/>
+    </row>
+    <row r="31" spans="1:15">
+      <c r="A31" s="3"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="7"/>
+      <c r="H31" s="5"/>
+      <c r="I31" s="7"/>
+      <c r="J31" s="5"/>
+      <c r="K31" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="L31" s="5"/>
+      <c r="M31" s="7"/>
+      <c r="N31" s="5"/>
+      <c r="O31" s="7"/>
+    </row>
+    <row r="32" spans="1:15">
+      <c r="A32" s="3"/>
+      <c r="B32" s="5"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="7"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="7"/>
+      <c r="H32" s="5"/>
+      <c r="I32" s="7"/>
+      <c r="J32" s="5"/>
+      <c r="K32" s="7"/>
+      <c r="L32" s="5"/>
+      <c r="M32" s="7"/>
+      <c r="N32" s="5"/>
+      <c r="O32" s="7"/>
+    </row>
+    <row r="33" spans="1:15">
+      <c r="A33" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="A8" s="6"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7" t="s">
+      <c r="B33" s="5"/>
+      <c r="C33" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D33" s="5"/>
+      <c r="E33" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F33" s="5"/>
+      <c r="G33" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H33" s="5"/>
+      <c r="I33" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J33" s="5"/>
+      <c r="K33" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="L33" s="5"/>
+      <c r="M33" s="6"/>
+      <c r="N33" s="5"/>
+      <c r="O33" s="6"/>
+    </row>
+    <row r="34" spans="1:15">
+      <c r="A34" s="3"/>
+      <c r="B34" s="5"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F34" s="5"/>
+      <c r="G34" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H34" s="5"/>
+      <c r="I34" s="6"/>
+      <c r="J34" s="5"/>
+      <c r="K34" s="6"/>
+      <c r="L34" s="5"/>
+      <c r="M34" s="6"/>
+      <c r="N34" s="5"/>
+      <c r="O34" s="6"/>
+    </row>
+    <row r="35" spans="1:15">
+      <c r="A35" s="3"/>
+      <c r="B35" s="5"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="6"/>
+      <c r="F35" s="5"/>
+      <c r="G35" s="6"/>
+      <c r="H35" s="5"/>
+      <c r="I35" s="6"/>
+      <c r="J35" s="5"/>
+      <c r="K35" s="6"/>
+      <c r="L35" s="5"/>
+      <c r="M35" s="6"/>
+      <c r="N35" s="5"/>
+      <c r="O35" s="6"/>
+    </row>
+    <row r="36" spans="1:15">
+      <c r="A36" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="A9" s="6"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="A10" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3" t="s">
+      <c r="B36" s="5"/>
+      <c r="C36" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D36" s="5"/>
+      <c r="E36" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F36" s="5"/>
+      <c r="G36" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H36" s="5"/>
+      <c r="I36" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="J36" s="5"/>
+      <c r="K36" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="L36" s="5"/>
+      <c r="M36" s="7"/>
+      <c r="N36" s="5"/>
+      <c r="O36" s="7"/>
+    </row>
+    <row r="37" spans="1:15">
+      <c r="A37" s="3"/>
+      <c r="B37" s="5"/>
+      <c r="C37" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D37" s="5"/>
+      <c r="E37" s="7"/>
+      <c r="F37" s="5"/>
+      <c r="G37" s="7"/>
+      <c r="H37" s="5"/>
+      <c r="I37" s="7"/>
+      <c r="J37" s="5"/>
+      <c r="K37" s="7"/>
+      <c r="L37" s="5"/>
+      <c r="M37" s="7"/>
+      <c r="N37" s="5"/>
+      <c r="O37" s="7"/>
+    </row>
+    <row r="38" spans="1:15">
+      <c r="A38" s="3"/>
+      <c r="B38" s="5"/>
+      <c r="C38" s="7"/>
+      <c r="D38" s="5"/>
+      <c r="E38" s="7"/>
+      <c r="F38" s="5"/>
+      <c r="G38" s="7"/>
+      <c r="H38" s="5"/>
+      <c r="I38" s="7"/>
+      <c r="J38" s="5"/>
+      <c r="K38" s="7"/>
+      <c r="L38" s="5"/>
+      <c r="M38" s="7"/>
+      <c r="N38" s="5"/>
+      <c r="O38" s="7"/>
+    </row>
+    <row r="39" spans="1:15">
+      <c r="A39" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B39" s="5">
+        <v>19</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D39" s="5">
+        <v>20</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F39" s="5">
+        <v>21</v>
+      </c>
+      <c r="G39" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H39" s="5">
+        <v>22</v>
+      </c>
+      <c r="I39" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="J39" s="5">
+        <v>23</v>
+      </c>
+      <c r="K39" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="L39" s="5">
+        <v>24</v>
+      </c>
+      <c r="M39" s="6"/>
+      <c r="N39" s="5">
+        <v>25</v>
+      </c>
+      <c r="O39" s="6"/>
+    </row>
+    <row r="40" spans="1:15">
+      <c r="A40" s="8"/>
+      <c r="B40" s="5"/>
+      <c r="C40" s="6"/>
+      <c r="D40" s="5"/>
+      <c r="E40" s="6"/>
+      <c r="F40" s="5"/>
+      <c r="G40" s="6"/>
+      <c r="H40" s="5"/>
+      <c r="I40" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J40" s="5"/>
+      <c r="K40" s="6"/>
+      <c r="L40" s="5"/>
+      <c r="M40" s="6"/>
+      <c r="N40" s="5"/>
+      <c r="O40" s="6"/>
+    </row>
+    <row r="41" spans="1:15">
+      <c r="A41" s="8"/>
+      <c r="B41" s="5"/>
+      <c r="C41" s="6"/>
+      <c r="D41" s="5"/>
+      <c r="E41" s="6"/>
+      <c r="F41" s="5"/>
+      <c r="G41" s="6"/>
+      <c r="H41" s="5"/>
+      <c r="I41" s="6"/>
+      <c r="J41" s="5"/>
+      <c r="K41" s="6"/>
+      <c r="L41" s="5"/>
+      <c r="M41" s="6"/>
+      <c r="N41" s="5"/>
+      <c r="O41" s="6"/>
+    </row>
+    <row r="42" spans="1:15">
+      <c r="A42" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B42" s="5"/>
+      <c r="C42" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D42" s="5"/>
+      <c r="E42" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F42" s="5"/>
+      <c r="G42" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H42" s="5"/>
+      <c r="I42" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="J42" s="5"/>
+      <c r="K42" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="L42" s="5"/>
+      <c r="M42" s="7"/>
+      <c r="N42" s="5"/>
+      <c r="O42" s="7"/>
+    </row>
+    <row r="43" spans="1:15">
+      <c r="A43" s="8"/>
+      <c r="B43" s="5"/>
+      <c r="C43" s="7"/>
+      <c r="D43" s="5"/>
+      <c r="E43" s="7"/>
+      <c r="F43" s="5"/>
+      <c r="G43" s="7"/>
+      <c r="H43" s="5"/>
+      <c r="I43" s="7"/>
+      <c r="J43" s="5"/>
+      <c r="K43" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="L43" s="5"/>
+      <c r="M43" s="7"/>
+      <c r="N43" s="5"/>
+      <c r="O43" s="7"/>
+    </row>
+    <row r="44" spans="1:15">
+      <c r="A44" s="8"/>
+      <c r="B44" s="5"/>
+      <c r="C44" s="7"/>
+      <c r="D44" s="5"/>
+      <c r="E44" s="7"/>
+      <c r="F44" s="5"/>
+      <c r="G44" s="7"/>
+      <c r="H44" s="5"/>
+      <c r="I44" s="7"/>
+      <c r="J44" s="5"/>
+      <c r="K44" s="7"/>
+      <c r="L44" s="5"/>
+      <c r="M44" s="7"/>
+      <c r="N44" s="5"/>
+      <c r="O44" s="7"/>
+    </row>
+    <row r="45" spans="1:15">
+      <c r="A45" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B45" s="5"/>
+      <c r="C45" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D45" s="5"/>
+      <c r="E45" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F45" s="5"/>
+      <c r="G45" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H45" s="5"/>
+      <c r="I45" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J45" s="5"/>
+      <c r="K45" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="L45" s="5"/>
+      <c r="M45" s="6"/>
+      <c r="N45" s="5"/>
+      <c r="O45" s="6"/>
+    </row>
+    <row r="46" spans="1:15">
+      <c r="A46" s="8"/>
+      <c r="B46" s="5"/>
+      <c r="C46" s="6"/>
+      <c r="D46" s="5"/>
+      <c r="E46" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F46" s="5"/>
+      <c r="G46" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H46" s="5"/>
+      <c r="I46" s="6"/>
+      <c r="J46" s="5"/>
+      <c r="K46" s="6"/>
+      <c r="L46" s="5"/>
+      <c r="M46" s="6"/>
+      <c r="N46" s="5"/>
+      <c r="O46" s="6"/>
+    </row>
+    <row r="47" spans="1:15">
+      <c r="A47" s="8"/>
+      <c r="B47" s="5"/>
+      <c r="C47" s="6"/>
+      <c r="D47" s="5"/>
+      <c r="E47" s="6"/>
+      <c r="F47" s="5"/>
+      <c r="G47" s="6"/>
+      <c r="H47" s="5"/>
+      <c r="I47" s="6"/>
+      <c r="J47" s="5"/>
+      <c r="K47" s="6"/>
+      <c r="L47" s="5"/>
+      <c r="M47" s="6"/>
+      <c r="N47" s="5"/>
+      <c r="O47" s="6"/>
+    </row>
+    <row r="48" spans="1:15">
+      <c r="A48" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="B48" s="5"/>
+      <c r="C48" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D48" s="5"/>
+      <c r="E48" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F48" s="5"/>
+      <c r="G48" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H48" s="5"/>
+      <c r="I48" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="J48" s="5"/>
+      <c r="K48" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="L48" s="5"/>
+      <c r="M48" s="7"/>
+      <c r="N48" s="5"/>
+      <c r="O48" s="7"/>
+    </row>
+    <row r="49" spans="1:15">
+      <c r="A49" s="8"/>
+      <c r="B49" s="5"/>
+      <c r="C49" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D49" s="5"/>
+      <c r="E49" s="7"/>
+      <c r="F49" s="5"/>
+      <c r="G49" s="7"/>
+      <c r="H49" s="5"/>
+      <c r="I49" s="7"/>
+      <c r="J49" s="5"/>
+      <c r="K49" s="7"/>
+      <c r="L49" s="5"/>
+      <c r="M49" s="7"/>
+      <c r="N49" s="5"/>
+      <c r="O49" s="7"/>
+    </row>
+    <row r="50" spans="1:15">
+      <c r="A50" s="8"/>
+      <c r="B50" s="5"/>
+      <c r="C50" s="7"/>
+      <c r="D50" s="5"/>
+      <c r="E50" s="7"/>
+      <c r="F50" s="5"/>
+      <c r="G50" s="7"/>
+      <c r="H50" s="5"/>
+      <c r="I50" s="7"/>
+      <c r="J50" s="5"/>
+      <c r="K50" s="7"/>
+      <c r="L50" s="5"/>
+      <c r="M50" s="7"/>
+      <c r="N50" s="5"/>
+      <c r="O50" s="7"/>
+    </row>
+    <row r="51" spans="1:15">
+      <c r="A51" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B51" s="5">
+        <v>26</v>
+      </c>
+      <c r="C51" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D51" s="5">
+        <v>27</v>
+      </c>
+      <c r="E51" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F51" s="5">
+        <v>28</v>
+      </c>
+      <c r="G51" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H51" s="5">
+        <v>29</v>
+      </c>
+      <c r="I51" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="J51" s="5">
+        <v>30</v>
+      </c>
+      <c r="K51" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="L51" s="5">
+        <v>31</v>
+      </c>
+      <c r="M51" s="6"/>
+      <c r="N51" s="4"/>
+      <c r="O51" s="4"/>
+    </row>
+    <row r="52" spans="1:15">
+      <c r="A52" s="3"/>
+      <c r="B52" s="5"/>
+      <c r="C52" s="6"/>
+      <c r="D52" s="5"/>
+      <c r="E52" s="6"/>
+      <c r="F52" s="5"/>
+      <c r="G52" s="6"/>
+      <c r="H52" s="5"/>
+      <c r="I52" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J52" s="5"/>
+      <c r="K52" s="6"/>
+      <c r="L52" s="5"/>
+      <c r="M52" s="6"/>
+      <c r="N52" s="4"/>
+      <c r="O52" s="4"/>
+    </row>
+    <row r="53" spans="1:15">
+      <c r="A53" s="3"/>
+      <c r="B53" s="5"/>
+      <c r="C53" s="6"/>
+      <c r="D53" s="5"/>
+      <c r="E53" s="6"/>
+      <c r="F53" s="5"/>
+      <c r="G53" s="6"/>
+      <c r="H53" s="5"/>
+      <c r="I53" s="6"/>
+      <c r="J53" s="5"/>
+      <c r="K53" s="6"/>
+      <c r="L53" s="5"/>
+      <c r="M53" s="6"/>
+      <c r="N53" s="4"/>
+      <c r="O53" s="4"/>
+    </row>
+    <row r="54" spans="1:15">
+      <c r="A54" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B54" s="5"/>
+      <c r="C54" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D54" s="5"/>
+      <c r="E54" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F54" s="5"/>
+      <c r="G54" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H54" s="5"/>
+      <c r="I54" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="J54" s="5"/>
+      <c r="K54" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="L54" s="5"/>
+      <c r="M54" s="7"/>
+      <c r="N54" s="4"/>
+      <c r="O54" s="4"/>
+    </row>
+    <row r="55" spans="1:15">
+      <c r="A55" s="3"/>
+      <c r="B55" s="5"/>
+      <c r="C55" s="7"/>
+      <c r="D55" s="5"/>
+      <c r="E55" s="7"/>
+      <c r="F55" s="5"/>
+      <c r="G55" s="7"/>
+      <c r="H55" s="5"/>
+      <c r="I55" s="7"/>
+      <c r="J55" s="5"/>
+      <c r="K55" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="L55" s="5"/>
+      <c r="M55" s="7"/>
+      <c r="N55" s="4"/>
+      <c r="O55" s="4"/>
+    </row>
+    <row r="56" spans="1:15">
+      <c r="A56" s="3"/>
+      <c r="B56" s="5"/>
+      <c r="C56" s="7"/>
+      <c r="D56" s="5"/>
+      <c r="E56" s="7"/>
+      <c r="F56" s="5"/>
+      <c r="G56" s="7"/>
+      <c r="H56" s="5"/>
+      <c r="I56" s="7"/>
+      <c r="J56" s="5"/>
+      <c r="K56" s="7"/>
+      <c r="L56" s="5"/>
+      <c r="M56" s="7"/>
+      <c r="N56" s="4"/>
+      <c r="O56" s="4"/>
+    </row>
+    <row r="57" spans="1:15">
+      <c r="A57" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B57" s="5"/>
+      <c r="C57" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D57" s="5"/>
+      <c r="E57" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F57" s="5"/>
+      <c r="G57" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H57" s="5"/>
+      <c r="I57" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J57" s="5"/>
+      <c r="K57" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="L57" s="5"/>
+      <c r="M57" s="6"/>
+      <c r="N57" s="4"/>
+      <c r="O57" s="4"/>
+    </row>
+    <row r="58" spans="1:15">
+      <c r="A58" s="3"/>
+      <c r="B58" s="5"/>
+      <c r="C58" s="6"/>
+      <c r="D58" s="5"/>
+      <c r="E58" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F58" s="5"/>
+      <c r="G58" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H58" s="5"/>
+      <c r="I58" s="6"/>
+      <c r="J58" s="5"/>
+      <c r="K58" s="6"/>
+      <c r="L58" s="5"/>
+      <c r="M58" s="6"/>
+      <c r="N58" s="4"/>
+      <c r="O58" s="4"/>
+    </row>
+    <row r="59" spans="1:15">
+      <c r="A59" s="3"/>
+      <c r="B59" s="5"/>
+      <c r="C59" s="6"/>
+      <c r="D59" s="5"/>
+      <c r="E59" s="6"/>
+      <c r="F59" s="5"/>
+      <c r="G59" s="6"/>
+      <c r="H59" s="5"/>
+      <c r="I59" s="6"/>
+      <c r="J59" s="5"/>
+      <c r="K59" s="6"/>
+      <c r="L59" s="5"/>
+      <c r="M59" s="6"/>
+      <c r="N59" s="4"/>
+      <c r="O59" s="4"/>
+    </row>
+    <row r="60" spans="1:15">
+      <c r="A60" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="A11" s="5"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="A12" s="5"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-    </row>
-    <row r="13" spans="1:9">
-      <c r="A13" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-    </row>
-    <row r="14" spans="1:9">
-      <c r="A14" s="6"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
-    </row>
-    <row r="15" spans="1:9">
-      <c r="A15" s="6"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
-    </row>
-    <row r="16" spans="1:9" ht="24" customHeight="1">
-      <c r="B16" s="4">
-        <v>5</v>
-      </c>
-      <c r="C16" s="4">
-        <v>6</v>
-      </c>
-      <c r="D16" s="4">
-        <v>7</v>
-      </c>
-      <c r="E16" s="4">
-        <v>8</v>
-      </c>
-      <c r="F16" s="4">
-        <v>9</v>
-      </c>
-      <c r="G16" s="4">
-        <v>10</v>
-      </c>
-      <c r="H16" s="4">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8">
-      <c r="A17" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-    </row>
-    <row r="18" spans="1:8">
-      <c r="A18" s="5"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-    </row>
-    <row r="19" spans="1:8">
-      <c r="A19" s="5"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-    </row>
-    <row r="20" spans="1:8">
-      <c r="A20" s="6" t="s">
+      <c r="B60" s="5"/>
+      <c r="C60" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B20" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E20" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F20" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
-    </row>
-    <row r="21" spans="1:8">
-      <c r="A21" s="6"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="G21" s="7"/>
-      <c r="H21" s="7"/>
-    </row>
-    <row r="22" spans="1:8">
-      <c r="A22" s="6"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="7"/>
-      <c r="H22" s="7"/>
-    </row>
-    <row r="23" spans="1:8">
-      <c r="A23" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G23" s="3"/>
-      <c r="H23" s="3"/>
-    </row>
-    <row r="24" spans="1:8">
-      <c r="A24" s="5"/>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
-      <c r="H24" s="3"/>
-    </row>
-    <row r="25" spans="1:8">
-      <c r="A25" s="5"/>
-      <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
-      <c r="H25" s="3"/>
-    </row>
-    <row r="26" spans="1:8">
-      <c r="A26" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B26" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C26" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D26" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E26" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F26" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="G26" s="7"/>
-      <c r="H26" s="7"/>
-    </row>
-    <row r="27" spans="1:8">
-      <c r="A27" s="6"/>
-      <c r="B27" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C27" s="7"/>
-      <c r="D27" s="7"/>
-      <c r="E27" s="7"/>
-      <c r="F27" s="7"/>
-      <c r="G27" s="7"/>
-      <c r="H27" s="7"/>
-    </row>
-    <row r="28" spans="1:8">
-      <c r="A28" s="6"/>
-      <c r="B28" s="7"/>
-      <c r="C28" s="7"/>
-      <c r="D28" s="7"/>
-      <c r="E28" s="7"/>
-      <c r="F28" s="7"/>
-      <c r="G28" s="7"/>
-      <c r="H28" s="7"/>
-    </row>
-    <row r="29" spans="1:8" ht="24" customHeight="1">
-      <c r="B29" s="4">
-        <v>12</v>
-      </c>
-      <c r="C29" s="4">
-        <v>13</v>
-      </c>
-      <c r="D29" s="4">
-        <v>14</v>
-      </c>
-      <c r="E29" s="4">
-        <v>15</v>
-      </c>
-      <c r="F29" s="4">
-        <v>16</v>
-      </c>
-      <c r="G29" s="4">
-        <v>17</v>
-      </c>
-      <c r="H29" s="4">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8">
-      <c r="A30" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F30" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G30" s="3"/>
-      <c r="H30" s="3"/>
-    </row>
-    <row r="31" spans="1:8">
-      <c r="A31" s="5"/>
-      <c r="B31" s="3"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F31" s="3"/>
-      <c r="G31" s="3"/>
-      <c r="H31" s="3"/>
-    </row>
-    <row r="32" spans="1:8">
-      <c r="A32" s="5"/>
-      <c r="B32" s="3"/>
-      <c r="C32" s="3"/>
-      <c r="D32" s="3"/>
-      <c r="E32" s="3"/>
-      <c r="F32" s="3"/>
-      <c r="G32" s="3"/>
-      <c r="H32" s="3"/>
-    </row>
-    <row r="33" spans="1:8">
-      <c r="A33" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B33" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C33" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D33" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E33" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F33" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="G33" s="7"/>
-      <c r="H33" s="7"/>
-    </row>
-    <row r="34" spans="1:8">
-      <c r="A34" s="6"/>
-      <c r="B34" s="7"/>
-      <c r="C34" s="7"/>
-      <c r="D34" s="7"/>
-      <c r="E34" s="7"/>
-      <c r="F34" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="G34" s="7"/>
-      <c r="H34" s="7"/>
-    </row>
-    <row r="35" spans="1:8">
-      <c r="A35" s="6"/>
-      <c r="B35" s="7"/>
-      <c r="C35" s="7"/>
-      <c r="D35" s="7"/>
-      <c r="E35" s="7"/>
-      <c r="F35" s="7"/>
-      <c r="G35" s="7"/>
-      <c r="H35" s="7"/>
-    </row>
-    <row r="36" spans="1:8">
-      <c r="A36" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D36" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E36" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F36" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G36" s="3"/>
-      <c r="H36" s="3"/>
-    </row>
-    <row r="37" spans="1:8">
-      <c r="A37" s="5"/>
-      <c r="B37" s="3"/>
-      <c r="C37" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E37" s="3"/>
-      <c r="F37" s="3"/>
-      <c r="G37" s="3"/>
-      <c r="H37" s="3"/>
-    </row>
-    <row r="38" spans="1:8">
-      <c r="A38" s="5"/>
-      <c r="B38" s="3"/>
-      <c r="C38" s="3"/>
-      <c r="D38" s="3"/>
-      <c r="E38" s="3"/>
-      <c r="F38" s="3"/>
-      <c r="G38" s="3"/>
-      <c r="H38" s="3"/>
-    </row>
-    <row r="39" spans="1:8">
-      <c r="A39" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B39" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C39" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D39" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E39" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F39" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="G39" s="7"/>
-      <c r="H39" s="7"/>
-    </row>
-    <row r="40" spans="1:8">
-      <c r="A40" s="6"/>
-      <c r="B40" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C40" s="7"/>
-      <c r="D40" s="7"/>
-      <c r="E40" s="7"/>
-      <c r="F40" s="7"/>
-      <c r="G40" s="7"/>
-      <c r="H40" s="7"/>
-    </row>
-    <row r="41" spans="1:8">
-      <c r="A41" s="6"/>
-      <c r="B41" s="7"/>
-      <c r="C41" s="7"/>
-      <c r="D41" s="7"/>
-      <c r="E41" s="7"/>
-      <c r="F41" s="7"/>
-      <c r="G41" s="7"/>
-      <c r="H41" s="7"/>
-    </row>
-    <row r="42" spans="1:8" ht="24" customHeight="1">
-      <c r="B42" s="4">
-        <v>19</v>
-      </c>
-      <c r="C42" s="4">
-        <v>20</v>
-      </c>
-      <c r="D42" s="4">
-        <v>21</v>
-      </c>
-      <c r="E42" s="4">
-        <v>22</v>
-      </c>
-      <c r="F42" s="4">
-        <v>23</v>
-      </c>
-      <c r="G42" s="4">
-        <v>24</v>
-      </c>
-      <c r="H42" s="4">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8">
-      <c r="A43" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B43" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D43" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E43" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F43" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G43" s="3"/>
-      <c r="H43" s="3"/>
-    </row>
-    <row r="44" spans="1:8">
-      <c r="A44" s="5"/>
-      <c r="B44" s="3"/>
-      <c r="C44" s="3"/>
-      <c r="D44" s="3"/>
-      <c r="E44" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F44" s="3"/>
-      <c r="G44" s="3"/>
-      <c r="H44" s="3"/>
-    </row>
-    <row r="45" spans="1:8">
-      <c r="A45" s="5"/>
-      <c r="B45" s="3"/>
-      <c r="C45" s="3"/>
-      <c r="D45" s="3"/>
-      <c r="E45" s="3"/>
-      <c r="F45" s="3"/>
-      <c r="G45" s="3"/>
-      <c r="H45" s="3"/>
-    </row>
-    <row r="46" spans="1:8">
-      <c r="A46" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B46" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C46" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D46" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E46" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F46" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="G46" s="7"/>
-      <c r="H46" s="7"/>
-    </row>
-    <row r="47" spans="1:8">
-      <c r="A47" s="6"/>
-      <c r="B47" s="7"/>
-      <c r="C47" s="7"/>
-      <c r="D47" s="7"/>
-      <c r="E47" s="7"/>
-      <c r="F47" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="G47" s="7"/>
-      <c r="H47" s="7"/>
-    </row>
-    <row r="48" spans="1:8">
-      <c r="A48" s="6"/>
-      <c r="B48" s="7"/>
-      <c r="C48" s="7"/>
-      <c r="D48" s="7"/>
-      <c r="E48" s="7"/>
-      <c r="F48" s="7"/>
-      <c r="G48" s="7"/>
-      <c r="H48" s="7"/>
-    </row>
-    <row r="49" spans="1:8">
-      <c r="A49" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B49" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C49" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D49" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E49" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F49" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G49" s="3"/>
-      <c r="H49" s="3"/>
-    </row>
-    <row r="50" spans="1:8">
-      <c r="A50" s="5"/>
-      <c r="B50" s="3"/>
-      <c r="C50" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D50" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E50" s="3"/>
-      <c r="F50" s="3"/>
-      <c r="G50" s="3"/>
-      <c r="H50" s="3"/>
-    </row>
-    <row r="51" spans="1:8">
-      <c r="A51" s="5"/>
-      <c r="B51" s="3"/>
-      <c r="C51" s="3"/>
-      <c r="D51" s="3"/>
-      <c r="E51" s="3"/>
-      <c r="F51" s="3"/>
-      <c r="G51" s="3"/>
-      <c r="H51" s="3"/>
-    </row>
-    <row r="52" spans="1:8">
-      <c r="A52" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B52" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C52" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D52" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E52" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F52" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="G52" s="7"/>
-      <c r="H52" s="7"/>
-    </row>
-    <row r="53" spans="1:8">
-      <c r="A53" s="6"/>
-      <c r="B53" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C53" s="7"/>
-      <c r="D53" s="7"/>
-      <c r="E53" s="7"/>
-      <c r="F53" s="7"/>
-      <c r="G53" s="7"/>
-      <c r="H53" s="7"/>
-    </row>
-    <row r="54" spans="1:8">
-      <c r="A54" s="6"/>
-      <c r="B54" s="7"/>
-      <c r="C54" s="7"/>
-      <c r="D54" s="7"/>
-      <c r="E54" s="7"/>
-      <c r="F54" s="7"/>
-      <c r="G54" s="7"/>
-      <c r="H54" s="7"/>
-    </row>
-    <row r="55" spans="1:8" ht="24" customHeight="1">
-      <c r="B55" s="4">
-        <v>26</v>
-      </c>
-      <c r="C55" s="4">
-        <v>27</v>
-      </c>
-      <c r="D55" s="4">
-        <v>28</v>
-      </c>
-      <c r="E55" s="4">
-        <v>29</v>
-      </c>
-      <c r="F55" s="4">
-        <v>30</v>
-      </c>
-      <c r="G55" s="4">
-        <v>31</v>
-      </c>
-      <c r="H55" s="3"/>
-    </row>
-    <row r="56" spans="1:8">
-      <c r="A56" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B56" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C56" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D56" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E56" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F56" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G56" s="3"/>
-      <c r="H56" s="3"/>
-    </row>
-    <row r="57" spans="1:8">
-      <c r="A57" s="5"/>
-      <c r="B57" s="3"/>
-      <c r="C57" s="3"/>
-      <c r="D57" s="3"/>
-      <c r="E57" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F57" s="3"/>
-      <c r="G57" s="3"/>
-      <c r="H57" s="3"/>
-    </row>
-    <row r="58" spans="1:8">
-      <c r="A58" s="5"/>
-      <c r="B58" s="3"/>
-      <c r="C58" s="3"/>
-      <c r="D58" s="3"/>
-      <c r="E58" s="3"/>
-      <c r="F58" s="3"/>
-      <c r="G58" s="3"/>
-      <c r="H58" s="3"/>
-    </row>
-    <row r="59" spans="1:8">
-      <c r="A59" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B59" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C59" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D59" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E59" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F59" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="G59" s="7"/>
-      <c r="H59" s="7"/>
-    </row>
-    <row r="60" spans="1:8">
-      <c r="A60" s="6"/>
-      <c r="B60" s="7"/>
-      <c r="C60" s="7"/>
-      <c r="D60" s="7"/>
-      <c r="E60" s="7"/>
-      <c r="F60" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="G60" s="7"/>
-      <c r="H60" s="7"/>
-    </row>
-    <row r="61" spans="1:8">
-      <c r="A61" s="6"/>
-      <c r="B61" s="7"/>
-      <c r="C61" s="7"/>
-      <c r="D61" s="7"/>
+      <c r="D60" s="5"/>
+      <c r="E60" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F60" s="5"/>
+      <c r="G60" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H60" s="5"/>
+      <c r="I60" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="J60" s="5"/>
+      <c r="K60" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="L60" s="5"/>
+      <c r="M60" s="7"/>
+      <c r="N60" s="4"/>
+      <c r="O60" s="4"/>
+    </row>
+    <row r="61" spans="1:15">
+      <c r="A61" s="3"/>
+      <c r="B61" s="5"/>
+      <c r="C61" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D61" s="5"/>
       <c r="E61" s="7"/>
-      <c r="F61" s="7"/>
+      <c r="F61" s="5"/>
       <c r="G61" s="7"/>
-      <c r="H61" s="7"/>
-    </row>
-    <row r="62" spans="1:8">
-      <c r="A62" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B62" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C62" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D62" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E62" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F62" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G62" s="3"/>
-      <c r="H62" s="3"/>
-    </row>
-    <row r="63" spans="1:8">
-      <c r="A63" s="5"/>
-      <c r="B63" s="3"/>
-      <c r="C63" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D63" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E63" s="3"/>
-      <c r="F63" s="3"/>
-      <c r="G63" s="3"/>
-      <c r="H63" s="3"/>
-    </row>
-    <row r="64" spans="1:8">
-      <c r="A64" s="5"/>
-      <c r="B64" s="3"/>
-      <c r="C64" s="3"/>
-      <c r="D64" s="3"/>
-      <c r="E64" s="3"/>
-      <c r="F64" s="3"/>
-      <c r="G64" s="3"/>
-      <c r="H64" s="3"/>
-    </row>
-    <row r="65" spans="1:8">
-      <c r="A65" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B65" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C65" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D65" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E65" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F65" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="G65" s="7"/>
-      <c r="H65" s="7"/>
-    </row>
-    <row r="66" spans="1:8">
-      <c r="A66" s="6"/>
-      <c r="B66" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C66" s="7"/>
-      <c r="D66" s="7"/>
-      <c r="E66" s="7"/>
-      <c r="F66" s="7"/>
-      <c r="G66" s="7"/>
-      <c r="H66" s="7"/>
-    </row>
-    <row r="67" spans="1:8">
-      <c r="A67" s="6"/>
-      <c r="B67" s="7"/>
-      <c r="C67" s="7"/>
-      <c r="D67" s="7"/>
-      <c r="E67" s="7"/>
-      <c r="F67" s="7"/>
-      <c r="G67" s="7"/>
-      <c r="H67" s="7"/>
+      <c r="H61" s="5"/>
+      <c r="I61" s="7"/>
+      <c r="J61" s="5"/>
+      <c r="K61" s="7"/>
+      <c r="L61" s="5"/>
+      <c r="M61" s="7"/>
+      <c r="N61" s="4"/>
+      <c r="O61" s="4"/>
+    </row>
+    <row r="62" spans="1:15">
+      <c r="A62" s="3"/>
+      <c r="B62" s="5"/>
+      <c r="C62" s="7"/>
+      <c r="D62" s="5"/>
+      <c r="E62" s="7"/>
+      <c r="F62" s="5"/>
+      <c r="G62" s="7"/>
+      <c r="H62" s="5"/>
+      <c r="I62" s="7"/>
+      <c r="J62" s="5"/>
+      <c r="K62" s="7"/>
+      <c r="L62" s="5"/>
+      <c r="M62" s="7"/>
+      <c r="N62" s="4"/>
+      <c r="O62" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="21">
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A4:A6"/>
-    <mergeCell ref="A7:A9"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="A13:A15"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="A20:A22"/>
-    <mergeCell ref="A23:A25"/>
-    <mergeCell ref="A26:A28"/>
+  <mergeCells count="63">
+    <mergeCell ref="A1:O1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="B3:C14"/>
+    <mergeCell ref="D3:E14"/>
+    <mergeCell ref="F3:G14"/>
+    <mergeCell ref="H3:H14"/>
+    <mergeCell ref="J3:J14"/>
+    <mergeCell ref="L3:L14"/>
+    <mergeCell ref="N3:N14"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="B15:B26"/>
+    <mergeCell ref="D15:D26"/>
+    <mergeCell ref="F15:F26"/>
+    <mergeCell ref="H15:H26"/>
+    <mergeCell ref="J15:J26"/>
+    <mergeCell ref="L15:L26"/>
+    <mergeCell ref="N15:N26"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="A21:A23"/>
+    <mergeCell ref="A24:A26"/>
+    <mergeCell ref="B27:B38"/>
+    <mergeCell ref="D27:D38"/>
+    <mergeCell ref="F27:F38"/>
+    <mergeCell ref="H27:H38"/>
+    <mergeCell ref="J27:J38"/>
+    <mergeCell ref="L27:L38"/>
+    <mergeCell ref="N27:N38"/>
+    <mergeCell ref="A27:A29"/>
     <mergeCell ref="A30:A32"/>
     <mergeCell ref="A33:A35"/>
     <mergeCell ref="A36:A38"/>
+    <mergeCell ref="B39:B50"/>
+    <mergeCell ref="D39:D50"/>
+    <mergeCell ref="F39:F50"/>
+    <mergeCell ref="H39:H50"/>
+    <mergeCell ref="J39:J50"/>
+    <mergeCell ref="L39:L50"/>
+    <mergeCell ref="N39:N50"/>
     <mergeCell ref="A39:A41"/>
-    <mergeCell ref="A43:A45"/>
-    <mergeCell ref="A46:A48"/>
-    <mergeCell ref="A49:A51"/>
-    <mergeCell ref="A52:A54"/>
-    <mergeCell ref="A56:A58"/>
-    <mergeCell ref="A59:A61"/>
-    <mergeCell ref="A62:A64"/>
-    <mergeCell ref="A65:A67"/>
+    <mergeCell ref="A42:A44"/>
+    <mergeCell ref="A45:A47"/>
+    <mergeCell ref="A48:A50"/>
+    <mergeCell ref="N51:O62"/>
+    <mergeCell ref="B51:B62"/>
+    <mergeCell ref="D51:D62"/>
+    <mergeCell ref="F51:F62"/>
+    <mergeCell ref="H51:H62"/>
+    <mergeCell ref="J51:J62"/>
+    <mergeCell ref="L51:L62"/>
+    <mergeCell ref="A51:A53"/>
+    <mergeCell ref="A54:A56"/>
+    <mergeCell ref="A57:A59"/>
+    <mergeCell ref="A60:A62"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2103,36 +2555,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="C1" s="9" t="s">
         <v>16</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B2">
         <v>22</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B3">
         <v>88</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -2152,1773 +2604,1773 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="C1" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="8" t="s">
-        <v>22</v>
-      </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="C2" s="10" t="s">
         <v>21</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B10" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C10" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C11" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B12" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B13" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C13" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B14" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B15" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C15" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B16" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C16" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B17" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B18" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C18" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B19" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C19" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B20" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C20" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B21" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C21" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B22" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C22" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B23" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C23" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B24" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C24" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B25" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C25" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B26" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C26" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B27" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C27" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B28" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C28" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C29" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C30" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C31" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B32" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C32" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B33" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C33" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B34" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C34" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B35" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C35" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B36" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C36" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B37" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C37" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B38" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C38" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B39" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C39" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B40" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C40" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B41" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C41" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B42" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C42" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B43" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C43" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B44" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C44" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B45" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C45" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B46" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C46" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B47" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C47" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B48" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C48" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B49" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C49" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B50" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C50" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="51" spans="1:3">
       <c r="A51" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B51" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C51" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B52" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C52" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="53" spans="1:3">
       <c r="A53" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B53" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C53" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="54" spans="1:3">
       <c r="A54" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B54" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C54" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="55" spans="1:3">
       <c r="A55" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B55" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C55" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="56" spans="1:3">
       <c r="A56" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B56" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C56" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="57" spans="1:3">
       <c r="A57" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B57" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C57" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="58" spans="1:3">
       <c r="A58" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B58" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C58" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="59" spans="1:3">
       <c r="A59" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B59" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C59" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="60" spans="1:3">
       <c r="A60" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B60" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C60" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="61" spans="1:3">
       <c r="A61" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B61" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C61" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="62" spans="1:3">
       <c r="A62" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B62" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C62" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="63" spans="1:3">
       <c r="A63" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B63" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C63" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="64" spans="1:3">
       <c r="A64" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B64" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C64" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="65" spans="1:3">
       <c r="A65" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B65" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C65" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="66" spans="1:3">
       <c r="A66" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B66" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C66" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="67" spans="1:3">
       <c r="A67" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B67" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C67" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="68" spans="1:3">
       <c r="A68" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B68" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C68" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="69" spans="1:3">
       <c r="A69" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B69" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C69" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="70" spans="1:3">
       <c r="A70" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B70" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C70" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="71" spans="1:3">
       <c r="A71" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B71" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C71" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="72" spans="1:3">
       <c r="A72" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B72" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C72" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="73" spans="1:3">
       <c r="A73" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B73" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C73" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="74" spans="1:3">
       <c r="A74" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B74" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C74" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="75" spans="1:3">
       <c r="A75" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B75" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C75" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="76" spans="1:3">
       <c r="A76" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B76" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C76" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="77" spans="1:3">
       <c r="A77" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B77" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C77" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="78" spans="1:3">
       <c r="A78" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B78" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C78" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="79" spans="1:3">
       <c r="A79" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B79" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C79" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="80" spans="1:3">
       <c r="A80" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B80" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C80" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="81" spans="1:3">
       <c r="A81" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B81" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C81" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="82" spans="1:3">
       <c r="A82" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B82" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C82" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="83" spans="1:3">
       <c r="A83" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B83" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C83" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="84" spans="1:3">
       <c r="A84" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B84" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C84" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="85" spans="1:3">
       <c r="A85" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B85" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C85" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="86" spans="1:3">
       <c r="A86" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B86" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C86" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="87" spans="1:3">
       <c r="A87" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B87" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C87" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="88" spans="1:3">
       <c r="A88" t="s">
+        <v>43</v>
+      </c>
+      <c r="B88" t="s">
+        <v>9</v>
+      </c>
+      <c r="C88" t="s">
         <v>44</v>
-      </c>
-      <c r="B88" t="s">
-        <v>12</v>
-      </c>
-      <c r="C88" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="89" spans="1:3">
       <c r="A89" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B89" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C89" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="90" spans="1:3">
       <c r="A90" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B90" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C90" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="92" spans="1:3">
       <c r="A92" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3">
+      <c r="A93" s="10" t="s">
         <v>46</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3">
-      <c r="A93" s="9" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="94" spans="1:3">
       <c r="A94" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="95" spans="1:3">
       <c r="A95" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="96" spans="1:3">
       <c r="A96" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="97" spans="1:1">
       <c r="A97" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="98" spans="1:1">
       <c r="A98" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="99" spans="1:1">
       <c r="A99" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="100" spans="1:1">
       <c r="A100" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="101" spans="1:1">
       <c r="A101" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="102" spans="1:1">
       <c r="A102" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="103" spans="1:1">
       <c r="A103" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="104" spans="1:1">
       <c r="A104" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="105" spans="1:1">
       <c r="A105" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="106" spans="1:1">
       <c r="A106" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="107" spans="1:1">
       <c r="A107" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="108" spans="1:1">
       <c r="A108" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="109" spans="1:1">
       <c r="A109" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="110" spans="1:1">
       <c r="A110" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="111" spans="1:1">
       <c r="A111" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="112" spans="1:1">
       <c r="A112" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="113" spans="1:1">
       <c r="A113" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="114" spans="1:1">
       <c r="A114" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="115" spans="1:1">
       <c r="A115" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="116" spans="1:1">
       <c r="A116" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="117" spans="1:1">
       <c r="A117" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="118" spans="1:1">
       <c r="A118" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="119" spans="1:1">
       <c r="A119" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="120" spans="1:1">
       <c r="A120" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="121" spans="1:1">
       <c r="A121" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="122" spans="1:1">
       <c r="A122" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="123" spans="1:1">
       <c r="A123" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="124" spans="1:1">
       <c r="A124" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="125" spans="1:1">
       <c r="A125" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="126" spans="1:1">
       <c r="A126" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="127" spans="1:1">
       <c r="A127" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="128" spans="1:1">
       <c r="A128" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="129" spans="1:1">
       <c r="A129" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="130" spans="1:1">
       <c r="A130" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="131" spans="1:1">
       <c r="A131" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="132" spans="1:1">
       <c r="A132" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="133" spans="1:1">
       <c r="A133" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="134" spans="1:1">
       <c r="A134" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="135" spans="1:1">
       <c r="A135" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="136" spans="1:1">
       <c r="A136" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="137" spans="1:1">
       <c r="A137" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="138" spans="1:1">
       <c r="A138" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="139" spans="1:1">
       <c r="A139" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="140" spans="1:1">
       <c r="A140" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="141" spans="1:1">
       <c r="A141" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="142" spans="1:1">
       <c r="A142" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="143" spans="1:1">
       <c r="A143" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="144" spans="1:1">
       <c r="A144" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="145" spans="1:1">
       <c r="A145" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="146" spans="1:1">
       <c r="A146" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="147" spans="1:1">
       <c r="A147" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="148" spans="1:1">
       <c r="A148" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="149" spans="1:1">
       <c r="A149" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="150" spans="1:1">
       <c r="A150" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="151" spans="1:1">
       <c r="A151" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="152" spans="1:1">
       <c r="A152" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="153" spans="1:1">
       <c r="A153" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="154" spans="1:1">
       <c r="A154" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="155" spans="1:1">
       <c r="A155" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="156" spans="1:1">
       <c r="A156" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="157" spans="1:1">
       <c r="A157" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="158" spans="1:1">
       <c r="A158" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="159" spans="1:1">
       <c r="A159" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="160" spans="1:1">
       <c r="A160" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="161" spans="1:1">
       <c r="A161" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="162" spans="1:1">
       <c r="A162" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="163" spans="1:1">
       <c r="A163" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="164" spans="1:1">
       <c r="A164" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="165" spans="1:1">
       <c r="A165" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="166" spans="1:1">
       <c r="A166" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="167" spans="1:1">
       <c r="A167" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="168" spans="1:1">
       <c r="A168" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="169" spans="1:1">
       <c r="A169" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="170" spans="1:1">
       <c r="A170" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="171" spans="1:1">
       <c r="A171" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="172" spans="1:1">
       <c r="A172" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="173" spans="1:1">
       <c r="A173" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="174" spans="1:1">
       <c r="A174" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="175" spans="1:1">
       <c r="A175" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="176" spans="1:1">
       <c r="A176" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="177" spans="1:1">
       <c r="A177" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="178" spans="1:1">
       <c r="A178" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="179" spans="1:1">
       <c r="A179" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="180" spans="1:1">
       <c r="A180" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="181" spans="1:1">
       <c r="A181" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="182" spans="1:1">
       <c r="A182" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="183" spans="1:1">
       <c r="A183" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="184" spans="1:1">
       <c r="A184" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="185" spans="1:1">
       <c r="A185" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="186" spans="1:1">
       <c r="A186" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="187" spans="1:1">
       <c r="A187" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="188" spans="1:1">
       <c r="A188" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="189" spans="1:1">
       <c r="A189" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="190" spans="1:1">
       <c r="A190" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="191" spans="1:1">
       <c r="A191" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="192" spans="1:1">
       <c r="A192" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="193" spans="1:1">
       <c r="A193" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="194" spans="1:1">
       <c r="A194" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="195" spans="1:1">
       <c r="A195" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="196" spans="1:1">
       <c r="A196" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="197" spans="1:1">
       <c r="A197" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="198" spans="1:1">
       <c r="A198" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="199" spans="1:1">
       <c r="A199" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="200" spans="1:1">
       <c r="A200" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="201" spans="1:1">
       <c r="A201" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="202" spans="1:1">
       <c r="A202" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="203" spans="1:1">
       <c r="A203" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="204" spans="1:1">
       <c r="A204" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="205" spans="1:1">
       <c r="A205" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="206" spans="1:1">
       <c r="A206" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="207" spans="1:1">
       <c r="A207" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="208" spans="1:1">
       <c r="A208" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="209" spans="1:1">
       <c r="A209" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="210" spans="1:1">
       <c r="A210" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="211" spans="1:1">
       <c r="A211" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="212" spans="1:1">
       <c r="A212" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="213" spans="1:1">
       <c r="A213" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="214" spans="1:1">
       <c r="A214" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="215" spans="1:1">
       <c r="A215" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="216" spans="1:1">
       <c r="A216" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="217" spans="1:1">
       <c r="A217" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="218" spans="1:1">
       <c r="A218" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="219" spans="1:1">
       <c r="A219" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="220" spans="1:1">
       <c r="A220" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="221" spans="1:1">
       <c r="A221" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="222" spans="1:1">
       <c r="A222" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="223" spans="1:1">
       <c r="A223" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="224" spans="1:1">
       <c r="A224" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="225" spans="1:1">
       <c r="A225" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="226" spans="1:1">
       <c r="A226" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="227" spans="1:1">
       <c r="A227" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="228" spans="1:1">
       <c r="A228" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="229" spans="1:1">
       <c r="A229" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="230" spans="1:1">
       <c r="A230" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="231" spans="1:1">
       <c r="A231" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="232" spans="1:1">
       <c r="A232" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="233" spans="1:1">
       <c r="A233" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="234" spans="1:1">
       <c r="A234" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="235" spans="1:1">
       <c r="A235" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="236" spans="1:1">
       <c r="A236" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="237" spans="1:1">
       <c r="A237" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="238" spans="1:1">
       <c r="A238" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="239" spans="1:1">
       <c r="A239" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="240" spans="1:1">
       <c r="A240" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="241" spans="1:1">
       <c r="A241" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="242" spans="1:1">
       <c r="A242" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="243" spans="1:1">
       <c r="A243" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="244" spans="1:1">
       <c r="A244" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="245" spans="1:1">
       <c r="A245" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="246" spans="1:1">
       <c r="A246" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="247" spans="1:1">
       <c r="A247" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add ics calendar integration
</commit_message>
<xml_diff>
--- a/schedule_5_2025.xlsx
+++ b/schedule_5_2025.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="198">
   <si>
     <t>May 2025</t>
   </si>
@@ -64,15 +64,6 @@
   </si>
   <si>
     <t>Total Shifts</t>
-  </si>
-  <si>
-    <t>Assignments</t>
-  </si>
-  <si>
-    <t>2025-05-01 9AM-11AM; 2025-05-02 11AM-1PM; 2025-05-05 3PM-5PM; 2025-05-06 1PM-3PM; 2025-05-07 1PM-3PM; 2025-05-08 9AM-11AM; 2025-05-09 11AM-1PM; 2025-05-12 3PM-5PM; 2025-05-13 1PM-3PM; 2025-05-14 1PM-3PM; 2025-05-15 9AM-11AM; 2025-05-16 11AM-1PM; 2025-05-19 3PM-5PM; 2025-05-20 1PM-3PM; 2025-05-21 1PM-3PM; 2025-05-22 9AM-11AM; 2025-05-23 11AM-1PM; 2025-05-26 3PM-5PM; 2025-05-27 1PM-3PM; 2025-05-28 1PM-3PM; 2025-05-29 9AM-11AM; 2025-05-30 11AM-1PM</t>
-  </si>
-  <si>
-    <t>2025-05-01 9AM-11AM; 2025-05-01 11AM-1PM; 2025-05-01 1PM-3PM; 2025-05-01 3PM-5PM; 2025-05-02 9AM-11AM; 2025-05-02 11AM-1PM; 2025-05-02 1PM-3PM; 2025-05-02 3PM-5PM; 2025-05-05 9AM-11AM; 2025-05-05 11AM-1PM; 2025-05-05 1PM-3PM; 2025-05-05 3PM-5PM; 2025-05-06 9AM-11AM; 2025-05-06 11AM-1PM; 2025-05-06 1PM-3PM; 2025-05-06 3PM-5PM; 2025-05-07 9AM-11AM; 2025-05-07 11AM-1PM; 2025-05-07 1PM-3PM; 2025-05-07 3PM-5PM; 2025-05-08 9AM-11AM; 2025-05-08 11AM-1PM; 2025-05-08 1PM-3PM; 2025-05-08 3PM-5PM; 2025-05-09 9AM-11AM; 2025-05-09 11AM-1PM; 2025-05-09 1PM-3PM; 2025-05-09 3PM-5PM; 2025-05-12 9AM-11AM; 2025-05-12 11AM-1PM; 2025-05-12 1PM-3PM; 2025-05-12 3PM-5PM; 2025-05-13 9AM-11AM; 2025-05-13 11AM-1PM; 2025-05-13 1PM-3PM; 2025-05-13 3PM-5PM; 2025-05-14 9AM-11AM; 2025-05-14 11AM-1PM; 2025-05-14 1PM-3PM; 2025-05-14 3PM-5PM; 2025-05-15 9AM-11AM; 2025-05-15 11AM-1PM; 2025-05-15 1PM-3PM; 2025-05-15 3PM-5PM; 2025-05-16 9AM-11AM; 2025-05-16 11AM-1PM; 2025-05-16 1PM-3PM; 2025-05-16 3PM-5PM; 2025-05-19 9AM-11AM; 2025-05-19 11AM-1PM; 2025-05-19 1PM-3PM; 2025-05-19 3PM-5PM; 2025-05-20 9AM-11AM; 2025-05-20 11AM-1PM; 2025-05-20 1PM-3PM; 2025-05-20 3PM-5PM; 2025-05-21 9AM-11AM; 2025-05-21 11AM-1PM; 2025-05-21 1PM-3PM; 2025-05-21 3PM-5PM; 2025-05-22 9AM-11AM; 2025-05-22 11AM-1PM; 2025-05-22 1PM-3PM; 2025-05-22 3PM-5PM; 2025-05-23 9AM-11AM; 2025-05-23 11AM-1PM; 2025-05-23 1PM-3PM; 2025-05-23 3PM-5PM; 2025-05-26 9AM-11AM; 2025-05-26 11AM-1PM; 2025-05-26 1PM-3PM; 2025-05-26 3PM-5PM; 2025-05-27 9AM-11AM; 2025-05-27 11AM-1PM; 2025-05-27 1PM-3PM; 2025-05-27 3PM-5PM; 2025-05-28 9AM-11AM; 2025-05-28 11AM-1PM; 2025-05-28 1PM-3PM; 2025-05-28 3PM-5PM; 2025-05-29 9AM-11AM; 2025-05-29 11AM-1PM; 2025-05-29 1PM-3PM; 2025-05-29 3PM-5PM; 2025-05-30 9AM-11AM; 2025-05-30 11AM-1PM; 2025-05-30 1PM-3PM; 2025-05-30 3PM-5PM</t>
   </si>
   <si>
     <t>Date</t>
@@ -735,7 +726,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -761,6 +752,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -2545,46 +2537,37 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="3" width="30.7109375" customWidth="1"/>
+    <col min="1" max="2" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:2">
       <c r="A1" s="9" t="s">
         <v>14</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
       <c r="B2">
         <v>22</v>
       </c>
-      <c r="C2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>13</v>
       </c>
       <c r="B3">
         <v>88</v>
-      </c>
-      <c r="C3" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -2604,41 +2587,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>21</v>
+      <c r="A1" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>21</v>
+      <c r="A2" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
@@ -2649,7 +2632,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
@@ -2660,7 +2643,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
@@ -2671,7 +2654,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B7" t="s">
         <v>8</v>
@@ -2682,18 +2665,18 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B8" t="s">
         <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B9" t="s">
         <v>10</v>
@@ -2704,7 +2687,7 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B10" t="s">
         <v>11</v>
@@ -2715,7 +2698,7 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B11" t="s">
         <v>8</v>
@@ -2726,7 +2709,7 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B12" t="s">
         <v>9</v>
@@ -2737,7 +2720,7 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B13" t="s">
         <v>10</v>
@@ -2748,18 +2731,18 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B14" t="s">
         <v>11</v>
       </c>
       <c r="C14" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B15" t="s">
         <v>8</v>
@@ -2770,7 +2753,7 @@
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B16" t="s">
         <v>9</v>
@@ -2781,18 +2764,18 @@
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B17" t="s">
         <v>10</v>
       </c>
       <c r="C17" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B18" t="s">
         <v>11</v>
@@ -2803,7 +2786,7 @@
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B19" t="s">
         <v>8</v>
@@ -2814,7 +2797,7 @@
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B20" t="s">
         <v>9</v>
@@ -2825,18 +2808,18 @@
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B21" t="s">
         <v>10</v>
       </c>
       <c r="C21" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B22" t="s">
         <v>11</v>
@@ -2847,18 +2830,18 @@
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B23" t="s">
         <v>8</v>
       </c>
       <c r="C23" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B24" t="s">
         <v>9</v>
@@ -2869,7 +2852,7 @@
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B25" t="s">
         <v>10</v>
@@ -2880,7 +2863,7 @@
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B26" t="s">
         <v>11</v>
@@ -2891,7 +2874,7 @@
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B27" t="s">
         <v>8</v>
@@ -2902,18 +2885,18 @@
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B28" t="s">
         <v>9</v>
       </c>
       <c r="C28" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B29" t="s">
         <v>10</v>
@@ -2924,7 +2907,7 @@
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B30" t="s">
         <v>11</v>
@@ -2935,7 +2918,7 @@
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B31" t="s">
         <v>8</v>
@@ -2946,7 +2929,7 @@
     </row>
     <row r="32" spans="1:3">
       <c r="A32" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B32" t="s">
         <v>9</v>
@@ -2957,7 +2940,7 @@
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B33" t="s">
         <v>10</v>
@@ -2968,18 +2951,18 @@
     </row>
     <row r="34" spans="1:3">
       <c r="A34" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B34" t="s">
         <v>11</v>
       </c>
       <c r="C34" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B35" t="s">
         <v>8</v>
@@ -2990,7 +2973,7 @@
     </row>
     <row r="36" spans="1:3">
       <c r="A36" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B36" t="s">
         <v>9</v>
@@ -3001,18 +2984,18 @@
     </row>
     <row r="37" spans="1:3">
       <c r="A37" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B37" t="s">
         <v>10</v>
       </c>
       <c r="C37" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B38" t="s">
         <v>11</v>
@@ -3023,7 +3006,7 @@
     </row>
     <row r="39" spans="1:3">
       <c r="A39" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B39" t="s">
         <v>8</v>
@@ -3034,7 +3017,7 @@
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B40" t="s">
         <v>9</v>
@@ -3045,18 +3028,18 @@
     </row>
     <row r="41" spans="1:3">
       <c r="A41" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B41" t="s">
         <v>10</v>
       </c>
       <c r="C41" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B42" t="s">
         <v>11</v>
@@ -3067,18 +3050,18 @@
     </row>
     <row r="43" spans="1:3">
       <c r="A43" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B43" t="s">
         <v>8</v>
       </c>
       <c r="C43" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B44" t="s">
         <v>9</v>
@@ -3089,7 +3072,7 @@
     </row>
     <row r="45" spans="1:3">
       <c r="A45" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B45" t="s">
         <v>10</v>
@@ -3100,7 +3083,7 @@
     </row>
     <row r="46" spans="1:3">
       <c r="A46" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B46" t="s">
         <v>11</v>
@@ -3111,7 +3094,7 @@
     </row>
     <row r="47" spans="1:3">
       <c r="A47" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B47" t="s">
         <v>8</v>
@@ -3122,18 +3105,18 @@
     </row>
     <row r="48" spans="1:3">
       <c r="A48" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B48" t="s">
         <v>9</v>
       </c>
       <c r="C48" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B49" t="s">
         <v>10</v>
@@ -3144,7 +3127,7 @@
     </row>
     <row r="50" spans="1:3">
       <c r="A50" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B50" t="s">
         <v>11</v>
@@ -3155,7 +3138,7 @@
     </row>
     <row r="51" spans="1:3">
       <c r="A51" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B51" t="s">
         <v>8</v>
@@ -3166,7 +3149,7 @@
     </row>
     <row r="52" spans="1:3">
       <c r="A52" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B52" t="s">
         <v>9</v>
@@ -3177,7 +3160,7 @@
     </row>
     <row r="53" spans="1:3">
       <c r="A53" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B53" t="s">
         <v>10</v>
@@ -3188,18 +3171,18 @@
     </row>
     <row r="54" spans="1:3">
       <c r="A54" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B54" t="s">
         <v>11</v>
       </c>
       <c r="C54" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="55" spans="1:3">
       <c r="A55" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B55" t="s">
         <v>8</v>
@@ -3210,7 +3193,7 @@
     </row>
     <row r="56" spans="1:3">
       <c r="A56" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B56" t="s">
         <v>9</v>
@@ -3221,18 +3204,18 @@
     </row>
     <row r="57" spans="1:3">
       <c r="A57" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B57" t="s">
         <v>10</v>
       </c>
       <c r="C57" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="58" spans="1:3">
       <c r="A58" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B58" t="s">
         <v>11</v>
@@ -3243,7 +3226,7 @@
     </row>
     <row r="59" spans="1:3">
       <c r="A59" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B59" t="s">
         <v>8</v>
@@ -3254,7 +3237,7 @@
     </row>
     <row r="60" spans="1:3">
       <c r="A60" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B60" t="s">
         <v>9</v>
@@ -3265,18 +3248,18 @@
     </row>
     <row r="61" spans="1:3">
       <c r="A61" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B61" t="s">
         <v>10</v>
       </c>
       <c r="C61" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="62" spans="1:3">
       <c r="A62" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B62" t="s">
         <v>11</v>
@@ -3287,18 +3270,18 @@
     </row>
     <row r="63" spans="1:3">
       <c r="A63" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B63" t="s">
         <v>8</v>
       </c>
       <c r="C63" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="64" spans="1:3">
       <c r="A64" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B64" t="s">
         <v>9</v>
@@ -3309,7 +3292,7 @@
     </row>
     <row r="65" spans="1:3">
       <c r="A65" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B65" t="s">
         <v>10</v>
@@ -3320,7 +3303,7 @@
     </row>
     <row r="66" spans="1:3">
       <c r="A66" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B66" t="s">
         <v>11</v>
@@ -3331,7 +3314,7 @@
     </row>
     <row r="67" spans="1:3">
       <c r="A67" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B67" t="s">
         <v>8</v>
@@ -3342,18 +3325,18 @@
     </row>
     <row r="68" spans="1:3">
       <c r="A68" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B68" t="s">
         <v>9</v>
       </c>
       <c r="C68" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="69" spans="1:3">
       <c r="A69" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B69" t="s">
         <v>10</v>
@@ -3364,7 +3347,7 @@
     </row>
     <row r="70" spans="1:3">
       <c r="A70" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B70" t="s">
         <v>11</v>
@@ -3375,7 +3358,7 @@
     </row>
     <row r="71" spans="1:3">
       <c r="A71" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B71" t="s">
         <v>8</v>
@@ -3386,7 +3369,7 @@
     </row>
     <row r="72" spans="1:3">
       <c r="A72" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B72" t="s">
         <v>9</v>
@@ -3397,7 +3380,7 @@
     </row>
     <row r="73" spans="1:3">
       <c r="A73" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B73" t="s">
         <v>10</v>
@@ -3408,18 +3391,18 @@
     </row>
     <row r="74" spans="1:3">
       <c r="A74" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B74" t="s">
         <v>11</v>
       </c>
       <c r="C74" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="75" spans="1:3">
       <c r="A75" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B75" t="s">
         <v>8</v>
@@ -3430,7 +3413,7 @@
     </row>
     <row r="76" spans="1:3">
       <c r="A76" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B76" t="s">
         <v>9</v>
@@ -3441,18 +3424,18 @@
     </row>
     <row r="77" spans="1:3">
       <c r="A77" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B77" t="s">
         <v>10</v>
       </c>
       <c r="C77" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="78" spans="1:3">
       <c r="A78" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B78" t="s">
         <v>11</v>
@@ -3463,7 +3446,7 @@
     </row>
     <row r="79" spans="1:3">
       <c r="A79" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B79" t="s">
         <v>8</v>
@@ -3474,7 +3457,7 @@
     </row>
     <row r="80" spans="1:3">
       <c r="A80" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B80" t="s">
         <v>9</v>
@@ -3485,18 +3468,18 @@
     </row>
     <row r="81" spans="1:3">
       <c r="A81" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B81" t="s">
         <v>10</v>
       </c>
       <c r="C81" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="82" spans="1:3">
       <c r="A82" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B82" t="s">
         <v>11</v>
@@ -3507,18 +3490,18 @@
     </row>
     <row r="83" spans="1:3">
       <c r="A83" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B83" t="s">
         <v>8</v>
       </c>
       <c r="C83" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="84" spans="1:3">
       <c r="A84" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B84" t="s">
         <v>9</v>
@@ -3529,7 +3512,7 @@
     </row>
     <row r="85" spans="1:3">
       <c r="A85" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B85" t="s">
         <v>10</v>
@@ -3540,7 +3523,7 @@
     </row>
     <row r="86" spans="1:3">
       <c r="A86" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B86" t="s">
         <v>11</v>
@@ -3551,7 +3534,7 @@
     </row>
     <row r="87" spans="1:3">
       <c r="A87" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B87" t="s">
         <v>8</v>
@@ -3562,18 +3545,18 @@
     </row>
     <row r="88" spans="1:3">
       <c r="A88" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B88" t="s">
         <v>9</v>
       </c>
       <c r="C88" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="89" spans="1:3">
       <c r="A89" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B89" t="s">
         <v>10</v>
@@ -3584,7 +3567,7 @@
     </row>
     <row r="90" spans="1:3">
       <c r="A90" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B90" t="s">
         <v>11</v>
@@ -3595,782 +3578,782 @@
     </row>
     <row r="92" spans="1:3">
       <c r="A92" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="93" spans="1:3">
-      <c r="A93" s="10" t="s">
-        <v>46</v>
+      <c r="A93" s="11" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="94" spans="1:3">
       <c r="A94" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="95" spans="1:3">
       <c r="A95" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="96" spans="1:3">
       <c r="A96" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="97" spans="1:1">
       <c r="A97" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="98" spans="1:1">
       <c r="A98" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="99" spans="1:1">
       <c r="A99" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="100" spans="1:1">
       <c r="A100" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="101" spans="1:1">
       <c r="A101" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="102" spans="1:1">
       <c r="A102" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="103" spans="1:1">
       <c r="A103" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="104" spans="1:1">
       <c r="A104" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="105" spans="1:1">
       <c r="A105" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="106" spans="1:1">
       <c r="A106" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="107" spans="1:1">
       <c r="A107" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="108" spans="1:1">
       <c r="A108" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="109" spans="1:1">
       <c r="A109" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="110" spans="1:1">
       <c r="A110" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="111" spans="1:1">
       <c r="A111" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="112" spans="1:1">
       <c r="A112" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="113" spans="1:1">
       <c r="A113" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="114" spans="1:1">
       <c r="A114" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="115" spans="1:1">
       <c r="A115" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="116" spans="1:1">
       <c r="A116" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="117" spans="1:1">
       <c r="A117" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="118" spans="1:1">
       <c r="A118" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="119" spans="1:1">
       <c r="A119" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="120" spans="1:1">
       <c r="A120" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="121" spans="1:1">
       <c r="A121" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="122" spans="1:1">
       <c r="A122" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="123" spans="1:1">
       <c r="A123" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="124" spans="1:1">
       <c r="A124" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="125" spans="1:1">
       <c r="A125" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="126" spans="1:1">
       <c r="A126" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="127" spans="1:1">
       <c r="A127" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="128" spans="1:1">
       <c r="A128" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="129" spans="1:1">
       <c r="A129" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="130" spans="1:1">
       <c r="A130" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="131" spans="1:1">
       <c r="A131" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="132" spans="1:1">
       <c r="A132" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="133" spans="1:1">
       <c r="A133" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="134" spans="1:1">
       <c r="A134" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="135" spans="1:1">
       <c r="A135" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="136" spans="1:1">
       <c r="A136" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="137" spans="1:1">
       <c r="A137" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="138" spans="1:1">
       <c r="A138" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="139" spans="1:1">
       <c r="A139" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="140" spans="1:1">
       <c r="A140" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="141" spans="1:1">
       <c r="A141" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="142" spans="1:1">
       <c r="A142" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="143" spans="1:1">
       <c r="A143" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="144" spans="1:1">
       <c r="A144" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="145" spans="1:1">
       <c r="A145" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="146" spans="1:1">
       <c r="A146" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="147" spans="1:1">
       <c r="A147" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="148" spans="1:1">
       <c r="A148" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="149" spans="1:1">
       <c r="A149" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="150" spans="1:1">
       <c r="A150" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="151" spans="1:1">
       <c r="A151" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="152" spans="1:1">
       <c r="A152" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="153" spans="1:1">
       <c r="A153" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="154" spans="1:1">
       <c r="A154" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="155" spans="1:1">
       <c r="A155" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="156" spans="1:1">
       <c r="A156" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="157" spans="1:1">
       <c r="A157" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="158" spans="1:1">
       <c r="A158" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="159" spans="1:1">
       <c r="A159" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="160" spans="1:1">
       <c r="A160" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="161" spans="1:1">
       <c r="A161" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="162" spans="1:1">
       <c r="A162" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="163" spans="1:1">
       <c r="A163" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="164" spans="1:1">
       <c r="A164" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="165" spans="1:1">
       <c r="A165" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="166" spans="1:1">
       <c r="A166" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="167" spans="1:1">
       <c r="A167" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="168" spans="1:1">
       <c r="A168" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="169" spans="1:1">
       <c r="A169" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="170" spans="1:1">
       <c r="A170" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="171" spans="1:1">
       <c r="A171" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="172" spans="1:1">
       <c r="A172" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="173" spans="1:1">
       <c r="A173" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="174" spans="1:1">
       <c r="A174" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="175" spans="1:1">
       <c r="A175" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="176" spans="1:1">
       <c r="A176" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="177" spans="1:1">
       <c r="A177" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="178" spans="1:1">
       <c r="A178" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="179" spans="1:1">
       <c r="A179" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="180" spans="1:1">
       <c r="A180" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="181" spans="1:1">
       <c r="A181" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="182" spans="1:1">
       <c r="A182" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="183" spans="1:1">
       <c r="A183" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="184" spans="1:1">
       <c r="A184" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="185" spans="1:1">
       <c r="A185" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="186" spans="1:1">
       <c r="A186" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="187" spans="1:1">
       <c r="A187" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="188" spans="1:1">
       <c r="A188" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="189" spans="1:1">
       <c r="A189" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="190" spans="1:1">
       <c r="A190" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="191" spans="1:1">
       <c r="A191" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="192" spans="1:1">
       <c r="A192" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="193" spans="1:1">
       <c r="A193" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="194" spans="1:1">
       <c r="A194" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="195" spans="1:1">
       <c r="A195" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="196" spans="1:1">
       <c r="A196" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="197" spans="1:1">
       <c r="A197" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="198" spans="1:1">
       <c r="A198" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="199" spans="1:1">
       <c r="A199" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="200" spans="1:1">
       <c r="A200" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="201" spans="1:1">
       <c r="A201" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="202" spans="1:1">
       <c r="A202" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="203" spans="1:1">
       <c r="A203" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="204" spans="1:1">
       <c r="A204" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="205" spans="1:1">
       <c r="A205" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="206" spans="1:1">
       <c r="A206" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="207" spans="1:1">
       <c r="A207" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="208" spans="1:1">
       <c r="A208" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="209" spans="1:1">
       <c r="A209" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="210" spans="1:1">
       <c r="A210" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="211" spans="1:1">
       <c r="A211" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="212" spans="1:1">
       <c r="A212" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="213" spans="1:1">
       <c r="A213" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="214" spans="1:1">
       <c r="A214" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="215" spans="1:1">
       <c r="A215" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="216" spans="1:1">
       <c r="A216" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="217" spans="1:1">
       <c r="A217" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="218" spans="1:1">
       <c r="A218" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="219" spans="1:1">
       <c r="A219" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="220" spans="1:1">
       <c r="A220" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="221" spans="1:1">
       <c r="A221" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="222" spans="1:1">
       <c r="A222" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="223" spans="1:1">
       <c r="A223" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="224" spans="1:1">
       <c r="A224" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="225" spans="1:1">
       <c r="A225" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="226" spans="1:1">
       <c r="A226" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="227" spans="1:1">
       <c r="A227" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="228" spans="1:1">
       <c r="A228" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="229" spans="1:1">
       <c r="A229" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="230" spans="1:1">
       <c r="A230" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="231" spans="1:1">
       <c r="A231" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="232" spans="1:1">
       <c r="A232" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="233" spans="1:1">
       <c r="A233" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="234" spans="1:1">
       <c r="A234" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="235" spans="1:1">
       <c r="A235" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="236" spans="1:1">
       <c r="A236" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="237" spans="1:1">
       <c r="A237" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="238" spans="1:1">
       <c r="A238" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="239" spans="1:1">
       <c r="A239" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="240" spans="1:1">
       <c r="A240" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="241" spans="1:1">
       <c r="A241" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="242" spans="1:1">
       <c r="A242" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="243" spans="1:1">
       <c r="A243" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="244" spans="1:1">
       <c r="A244" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
     <row r="245" spans="1:1">
       <c r="A245" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="246" spans="1:1">
       <c r="A246" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="247" spans="1:1">
       <c r="A247" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
implement calendar subscription service
</commit_message>
<xml_diff>
--- a/schedule_5_2025.xlsx
+++ b/schedule_5_2025.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="199">
   <si>
     <t>May 2025</t>
   </si>
@@ -67,12 +67,6 @@
   </si>
   <si>
     <t>Calendar URL</t>
-  </si>
-  <si>
-    <t>https://raw.githubusercontent.com/Meghanuni/smr_scheduler/main/ics/R_C.ics</t>
-  </si>
-  <si>
-    <t>https://raw.githubusercontent.com/Meghanuni/smr_scheduler/main/ics/b_b.ics</t>
   </si>
   <si>
     <t>Date</t>
@@ -676,8 +670,8 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
@@ -739,12 +733,8 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="top"/>
-      <protection locked="0"/>
-    </xf>
   </cellStyleXfs>
   <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -773,14 +763,13 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2565,8 +2554,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="1" max="2" width="20.7109375" customWidth="1"/>
     <col min="3" max="3" width="40.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2588,8 +2576,9 @@
       <c r="B2">
         <v>22</v>
       </c>
-      <c r="C2" s="10" t="s">
-        <v>17</v>
+      <c r="C2" s="10">
+        <f>HYPERLINK("webcal://meghanuni.github.io/smr_scheduler/ics/R_C.ics", "Subscribe")</f>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -2599,15 +2588,12 @@
       <c r="B3">
         <v>88</v>
       </c>
-      <c r="C3" s="10" t="s">
-        <v>18</v>
+      <c r="C3" s="10">
+        <f>HYPERLINK("webcal://meghanuni.github.io/smr_scheduler/ics/b_b.ics", "Subscribe")</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="C3" r:id="rId2"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2625,40 +2611,40 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="11" t="s">
         <v>19</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="12" t="s">
         <v>19</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
@@ -2669,7 +2655,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
@@ -2680,7 +2666,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
@@ -2691,7 +2677,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B7" t="s">
         <v>8</v>
@@ -2702,18 +2688,18 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B8" t="s">
         <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B9" t="s">
         <v>10</v>
@@ -2724,7 +2710,7 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B10" t="s">
         <v>11</v>
@@ -2735,7 +2721,7 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B11" t="s">
         <v>8</v>
@@ -2746,7 +2732,7 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B12" t="s">
         <v>9</v>
@@ -2757,7 +2743,7 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B13" t="s">
         <v>10</v>
@@ -2768,18 +2754,18 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B14" t="s">
         <v>11</v>
       </c>
       <c r="C14" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B15" t="s">
         <v>8</v>
@@ -2790,7 +2776,7 @@
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B16" t="s">
         <v>9</v>
@@ -2801,18 +2787,18 @@
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B17" t="s">
         <v>10</v>
       </c>
       <c r="C17" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B18" t="s">
         <v>11</v>
@@ -2823,7 +2809,7 @@
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B19" t="s">
         <v>8</v>
@@ -2834,7 +2820,7 @@
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B20" t="s">
         <v>9</v>
@@ -2845,18 +2831,18 @@
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B21" t="s">
         <v>10</v>
       </c>
       <c r="C21" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B22" t="s">
         <v>11</v>
@@ -2867,18 +2853,18 @@
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B23" t="s">
         <v>8</v>
       </c>
       <c r="C23" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B24" t="s">
         <v>9</v>
@@ -2889,7 +2875,7 @@
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B25" t="s">
         <v>10</v>
@@ -2900,7 +2886,7 @@
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B26" t="s">
         <v>11</v>
@@ -2911,7 +2897,7 @@
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B27" t="s">
         <v>8</v>
@@ -2922,18 +2908,18 @@
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B28" t="s">
         <v>9</v>
       </c>
       <c r="C28" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B29" t="s">
         <v>10</v>
@@ -2944,7 +2930,7 @@
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B30" t="s">
         <v>11</v>
@@ -2955,7 +2941,7 @@
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B31" t="s">
         <v>8</v>
@@ -2966,7 +2952,7 @@
     </row>
     <row r="32" spans="1:3">
       <c r="A32" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B32" t="s">
         <v>9</v>
@@ -2977,7 +2963,7 @@
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B33" t="s">
         <v>10</v>
@@ -2988,18 +2974,18 @@
     </row>
     <row r="34" spans="1:3">
       <c r="A34" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B34" t="s">
         <v>11</v>
       </c>
       <c r="C34" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B35" t="s">
         <v>8</v>
@@ -3010,7 +2996,7 @@
     </row>
     <row r="36" spans="1:3">
       <c r="A36" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B36" t="s">
         <v>9</v>
@@ -3021,18 +3007,18 @@
     </row>
     <row r="37" spans="1:3">
       <c r="A37" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B37" t="s">
         <v>10</v>
       </c>
       <c r="C37" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B38" t="s">
         <v>11</v>
@@ -3043,7 +3029,7 @@
     </row>
     <row r="39" spans="1:3">
       <c r="A39" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B39" t="s">
         <v>8</v>
@@ -3054,7 +3040,7 @@
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B40" t="s">
         <v>9</v>
@@ -3065,18 +3051,18 @@
     </row>
     <row r="41" spans="1:3">
       <c r="A41" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B41" t="s">
         <v>10</v>
       </c>
       <c r="C41" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B42" t="s">
         <v>11</v>
@@ -3087,18 +3073,18 @@
     </row>
     <row r="43" spans="1:3">
       <c r="A43" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B43" t="s">
         <v>8</v>
       </c>
       <c r="C43" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B44" t="s">
         <v>9</v>
@@ -3109,7 +3095,7 @@
     </row>
     <row r="45" spans="1:3">
       <c r="A45" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B45" t="s">
         <v>10</v>
@@ -3120,7 +3106,7 @@
     </row>
     <row r="46" spans="1:3">
       <c r="A46" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B46" t="s">
         <v>11</v>
@@ -3131,7 +3117,7 @@
     </row>
     <row r="47" spans="1:3">
       <c r="A47" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B47" t="s">
         <v>8</v>
@@ -3142,18 +3128,18 @@
     </row>
     <row r="48" spans="1:3">
       <c r="A48" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B48" t="s">
         <v>9</v>
       </c>
       <c r="C48" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B49" t="s">
         <v>10</v>
@@ -3164,7 +3150,7 @@
     </row>
     <row r="50" spans="1:3">
       <c r="A50" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B50" t="s">
         <v>11</v>
@@ -3175,7 +3161,7 @@
     </row>
     <row r="51" spans="1:3">
       <c r="A51" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B51" t="s">
         <v>8</v>
@@ -3186,7 +3172,7 @@
     </row>
     <row r="52" spans="1:3">
       <c r="A52" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B52" t="s">
         <v>9</v>
@@ -3197,7 +3183,7 @@
     </row>
     <row r="53" spans="1:3">
       <c r="A53" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B53" t="s">
         <v>10</v>
@@ -3208,18 +3194,18 @@
     </row>
     <row r="54" spans="1:3">
       <c r="A54" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B54" t="s">
         <v>11</v>
       </c>
       <c r="C54" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="55" spans="1:3">
       <c r="A55" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B55" t="s">
         <v>8</v>
@@ -3230,7 +3216,7 @@
     </row>
     <row r="56" spans="1:3">
       <c r="A56" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B56" t="s">
         <v>9</v>
@@ -3241,18 +3227,18 @@
     </row>
     <row r="57" spans="1:3">
       <c r="A57" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B57" t="s">
         <v>10</v>
       </c>
       <c r="C57" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="58" spans="1:3">
       <c r="A58" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B58" t="s">
         <v>11</v>
@@ -3263,7 +3249,7 @@
     </row>
     <row r="59" spans="1:3">
       <c r="A59" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B59" t="s">
         <v>8</v>
@@ -3274,7 +3260,7 @@
     </row>
     <row r="60" spans="1:3">
       <c r="A60" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B60" t="s">
         <v>9</v>
@@ -3285,18 +3271,18 @@
     </row>
     <row r="61" spans="1:3">
       <c r="A61" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B61" t="s">
         <v>10</v>
       </c>
       <c r="C61" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="62" spans="1:3">
       <c r="A62" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B62" t="s">
         <v>11</v>
@@ -3307,18 +3293,18 @@
     </row>
     <row r="63" spans="1:3">
       <c r="A63" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B63" t="s">
         <v>8</v>
       </c>
       <c r="C63" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="64" spans="1:3">
       <c r="A64" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B64" t="s">
         <v>9</v>
@@ -3329,7 +3315,7 @@
     </row>
     <row r="65" spans="1:3">
       <c r="A65" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B65" t="s">
         <v>10</v>
@@ -3340,7 +3326,7 @@
     </row>
     <row r="66" spans="1:3">
       <c r="A66" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B66" t="s">
         <v>11</v>
@@ -3351,7 +3337,7 @@
     </row>
     <row r="67" spans="1:3">
       <c r="A67" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B67" t="s">
         <v>8</v>
@@ -3362,18 +3348,18 @@
     </row>
     <row r="68" spans="1:3">
       <c r="A68" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B68" t="s">
         <v>9</v>
       </c>
       <c r="C68" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="69" spans="1:3">
       <c r="A69" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B69" t="s">
         <v>10</v>
@@ -3384,7 +3370,7 @@
     </row>
     <row r="70" spans="1:3">
       <c r="A70" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B70" t="s">
         <v>11</v>
@@ -3395,7 +3381,7 @@
     </row>
     <row r="71" spans="1:3">
       <c r="A71" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B71" t="s">
         <v>8</v>
@@ -3406,7 +3392,7 @@
     </row>
     <row r="72" spans="1:3">
       <c r="A72" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B72" t="s">
         <v>9</v>
@@ -3417,7 +3403,7 @@
     </row>
     <row r="73" spans="1:3">
       <c r="A73" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B73" t="s">
         <v>10</v>
@@ -3428,18 +3414,18 @@
     </row>
     <row r="74" spans="1:3">
       <c r="A74" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B74" t="s">
         <v>11</v>
       </c>
       <c r="C74" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="75" spans="1:3">
       <c r="A75" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B75" t="s">
         <v>8</v>
@@ -3450,7 +3436,7 @@
     </row>
     <row r="76" spans="1:3">
       <c r="A76" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B76" t="s">
         <v>9</v>
@@ -3461,18 +3447,18 @@
     </row>
     <row r="77" spans="1:3">
       <c r="A77" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B77" t="s">
         <v>10</v>
       </c>
       <c r="C77" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="78" spans="1:3">
       <c r="A78" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B78" t="s">
         <v>11</v>
@@ -3483,7 +3469,7 @@
     </row>
     <row r="79" spans="1:3">
       <c r="A79" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B79" t="s">
         <v>8</v>
@@ -3494,7 +3480,7 @@
     </row>
     <row r="80" spans="1:3">
       <c r="A80" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B80" t="s">
         <v>9</v>
@@ -3505,18 +3491,18 @@
     </row>
     <row r="81" spans="1:3">
       <c r="A81" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B81" t="s">
         <v>10</v>
       </c>
       <c r="C81" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="82" spans="1:3">
       <c r="A82" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B82" t="s">
         <v>11</v>
@@ -3527,18 +3513,18 @@
     </row>
     <row r="83" spans="1:3">
       <c r="A83" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B83" t="s">
         <v>8</v>
       </c>
       <c r="C83" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="84" spans="1:3">
       <c r="A84" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B84" t="s">
         <v>9</v>
@@ -3549,7 +3535,7 @@
     </row>
     <row r="85" spans="1:3">
       <c r="A85" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B85" t="s">
         <v>10</v>
@@ -3560,7 +3546,7 @@
     </row>
     <row r="86" spans="1:3">
       <c r="A86" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B86" t="s">
         <v>11</v>
@@ -3571,7 +3557,7 @@
     </row>
     <row r="87" spans="1:3">
       <c r="A87" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B87" t="s">
         <v>8</v>
@@ -3582,18 +3568,18 @@
     </row>
     <row r="88" spans="1:3">
       <c r="A88" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B88" t="s">
         <v>9</v>
       </c>
       <c r="C88" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="89" spans="1:3">
       <c r="A89" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B89" t="s">
         <v>10</v>
@@ -3604,7 +3590,7 @@
     </row>
     <row r="90" spans="1:3">
       <c r="A90" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B90" t="s">
         <v>11</v>
@@ -3615,782 +3601,782 @@
     </row>
     <row r="92" spans="1:3">
       <c r="A92" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="93" spans="1:3">
       <c r="A93" s="12" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="94" spans="1:3">
       <c r="A94" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="95" spans="1:3">
       <c r="A95" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="96" spans="1:3">
       <c r="A96" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="97" spans="1:1">
       <c r="A97" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="98" spans="1:1">
       <c r="A98" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="99" spans="1:1">
       <c r="A99" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="100" spans="1:1">
       <c r="A100" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="101" spans="1:1">
       <c r="A101" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="102" spans="1:1">
       <c r="A102" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="103" spans="1:1">
       <c r="A103" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="104" spans="1:1">
       <c r="A104" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="105" spans="1:1">
       <c r="A105" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="106" spans="1:1">
       <c r="A106" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="107" spans="1:1">
       <c r="A107" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="108" spans="1:1">
       <c r="A108" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="109" spans="1:1">
       <c r="A109" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="110" spans="1:1">
       <c r="A110" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="111" spans="1:1">
       <c r="A111" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="112" spans="1:1">
       <c r="A112" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="113" spans="1:1">
       <c r="A113" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="114" spans="1:1">
       <c r="A114" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="115" spans="1:1">
       <c r="A115" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="116" spans="1:1">
       <c r="A116" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="117" spans="1:1">
       <c r="A117" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="118" spans="1:1">
       <c r="A118" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="119" spans="1:1">
       <c r="A119" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="120" spans="1:1">
       <c r="A120" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="121" spans="1:1">
       <c r="A121" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="122" spans="1:1">
       <c r="A122" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="123" spans="1:1">
       <c r="A123" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="124" spans="1:1">
       <c r="A124" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="125" spans="1:1">
       <c r="A125" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="126" spans="1:1">
       <c r="A126" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="127" spans="1:1">
       <c r="A127" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="128" spans="1:1">
       <c r="A128" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="129" spans="1:1">
       <c r="A129" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="130" spans="1:1">
       <c r="A130" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="131" spans="1:1">
       <c r="A131" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="132" spans="1:1">
       <c r="A132" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="133" spans="1:1">
       <c r="A133" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="134" spans="1:1">
       <c r="A134" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="135" spans="1:1">
       <c r="A135" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="136" spans="1:1">
       <c r="A136" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="137" spans="1:1">
       <c r="A137" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="138" spans="1:1">
       <c r="A138" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="139" spans="1:1">
       <c r="A139" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="140" spans="1:1">
       <c r="A140" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="141" spans="1:1">
       <c r="A141" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="142" spans="1:1">
       <c r="A142" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="143" spans="1:1">
       <c r="A143" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="144" spans="1:1">
       <c r="A144" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="145" spans="1:1">
       <c r="A145" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="146" spans="1:1">
       <c r="A146" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="147" spans="1:1">
       <c r="A147" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="148" spans="1:1">
       <c r="A148" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="149" spans="1:1">
       <c r="A149" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="150" spans="1:1">
       <c r="A150" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="151" spans="1:1">
       <c r="A151" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="152" spans="1:1">
       <c r="A152" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="153" spans="1:1">
       <c r="A153" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="154" spans="1:1">
       <c r="A154" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="155" spans="1:1">
       <c r="A155" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="156" spans="1:1">
       <c r="A156" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="157" spans="1:1">
       <c r="A157" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="158" spans="1:1">
       <c r="A158" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="159" spans="1:1">
       <c r="A159" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="160" spans="1:1">
       <c r="A160" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="161" spans="1:1">
       <c r="A161" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="162" spans="1:1">
       <c r="A162" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="163" spans="1:1">
       <c r="A163" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="164" spans="1:1">
       <c r="A164" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="165" spans="1:1">
       <c r="A165" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="166" spans="1:1">
       <c r="A166" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="167" spans="1:1">
       <c r="A167" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="168" spans="1:1">
       <c r="A168" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="169" spans="1:1">
       <c r="A169" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="170" spans="1:1">
       <c r="A170" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="171" spans="1:1">
       <c r="A171" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="172" spans="1:1">
       <c r="A172" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="173" spans="1:1">
       <c r="A173" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="174" spans="1:1">
       <c r="A174" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="175" spans="1:1">
       <c r="A175" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="176" spans="1:1">
       <c r="A176" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="177" spans="1:1">
       <c r="A177" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="178" spans="1:1">
       <c r="A178" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="179" spans="1:1">
       <c r="A179" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="180" spans="1:1">
       <c r="A180" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="181" spans="1:1">
       <c r="A181" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="182" spans="1:1">
       <c r="A182" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="183" spans="1:1">
       <c r="A183" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="184" spans="1:1">
       <c r="A184" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="185" spans="1:1">
       <c r="A185" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="186" spans="1:1">
       <c r="A186" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="187" spans="1:1">
       <c r="A187" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="188" spans="1:1">
       <c r="A188" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="189" spans="1:1">
       <c r="A189" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="190" spans="1:1">
       <c r="A190" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="191" spans="1:1">
       <c r="A191" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="192" spans="1:1">
       <c r="A192" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="193" spans="1:1">
       <c r="A193" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="194" spans="1:1">
       <c r="A194" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="195" spans="1:1">
       <c r="A195" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="196" spans="1:1">
       <c r="A196" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="197" spans="1:1">
       <c r="A197" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="198" spans="1:1">
       <c r="A198" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="199" spans="1:1">
       <c r="A199" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="200" spans="1:1">
       <c r="A200" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="201" spans="1:1">
       <c r="A201" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="202" spans="1:1">
       <c r="A202" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="203" spans="1:1">
       <c r="A203" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="204" spans="1:1">
       <c r="A204" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="205" spans="1:1">
       <c r="A205" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="206" spans="1:1">
       <c r="A206" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="207" spans="1:1">
       <c r="A207" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="208" spans="1:1">
       <c r="A208" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="209" spans="1:1">
       <c r="A209" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="210" spans="1:1">
       <c r="A210" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="211" spans="1:1">
       <c r="A211" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="212" spans="1:1">
       <c r="A212" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="213" spans="1:1">
       <c r="A213" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="214" spans="1:1">
       <c r="A214" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="215" spans="1:1">
       <c r="A215" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="216" spans="1:1">
       <c r="A216" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="217" spans="1:1">
       <c r="A217" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="218" spans="1:1">
       <c r="A218" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="219" spans="1:1">
       <c r="A219" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="220" spans="1:1">
       <c r="A220" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="221" spans="1:1">
       <c r="A221" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="222" spans="1:1">
       <c r="A222" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="223" spans="1:1">
       <c r="A223" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="224" spans="1:1">
       <c r="A224" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="225" spans="1:1">
       <c r="A225" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="226" spans="1:1">
       <c r="A226" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="227" spans="1:1">
       <c r="A227" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="228" spans="1:1">
       <c r="A228" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="229" spans="1:1">
       <c r="A229" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="230" spans="1:1">
       <c r="A230" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="231" spans="1:1">
       <c r="A231" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="232" spans="1:1">
       <c r="A232" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="233" spans="1:1">
       <c r="A233" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="234" spans="1:1">
       <c r="A234" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="235" spans="1:1">
       <c r="A235" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="236" spans="1:1">
       <c r="A236" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="237" spans="1:1">
       <c r="A237" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="238" spans="1:1">
       <c r="A238" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="239" spans="1:1">
       <c r="A239" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="240" spans="1:1">
       <c r="A240" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="241" spans="1:1">
       <c r="A241" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="242" spans="1:1">
       <c r="A242" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="243" spans="1:1">
       <c r="A243" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="244" spans="1:1">
       <c r="A244" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="245" spans="1:1">
       <c r="A245" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="246" spans="1:1">
       <c r="A246" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="247" spans="1:1">
       <c r="A247" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
   </sheetData>

</xml_diff>